<commit_message>
Solved Problem 12 Lucky Number Constructive/Implementation
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA13074-75B4-4CFF-8213-8D8B166D551D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1346AD-EC2F-46ED-BA84-846AB44C8206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:D405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1738,7 +1738,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>6</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Solved Construcive / Implementation Problem
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083CA77A-6127-4055-A7BA-0B6E08C5B683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C4236A-139A-40E9-8AE4-E483DA73CEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1542,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D405"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1808,7 +1808,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>6</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1822,7 +1822,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>6</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1836,7 +1836,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>6</v>
+        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1850,7 +1850,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>6</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Solved Implementation And Constructive
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E832CC5-C63F-4C95-A875-829C57FF9697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDA96B5-D8DD-4838-AF6B-0E5B668D473B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,13 +184,7 @@
     <t>48. https://codeforces.com/problemset/problem/507/A</t>
   </si>
   <si>
-    <t>49. https://codeforces.com/problemset/problem/507/A</t>
-  </si>
-  <si>
     <t>50. https://codeforces.com/problemset/problem/486/B</t>
-  </si>
-  <si>
-    <t>1.https://codeforces.com/problemset/problem/282/A</t>
   </si>
   <si>
     <t>1. https://codeforces.com/problemset/problem/1337/A</t>
@@ -1073,6 +1067,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>1. https://codeforces.com/problemset/problem/282/A</t>
+  </si>
+  <si>
+    <t>49. https://codeforces.com/problemset/problem/1237/A</t>
   </si>
 </sst>
 </file>
@@ -1542,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1581,10 +1581,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>56</v>
+        <v>339</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1598,7 +1598,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1612,7 +1612,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1626,7 +1626,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1640,7 +1640,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1654,7 +1654,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1668,7 +1668,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1682,7 +1682,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1696,7 +1696,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1710,7 +1710,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1738,7 +1738,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1752,7 +1752,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1766,7 +1766,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1780,7 +1780,7 @@
         <v>20</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1794,7 +1794,7 @@
         <v>21</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1808,7 +1808,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1822,7 +1822,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1836,7 +1836,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1850,7 +1850,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1864,7 +1864,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1878,7 +1878,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1892,7 +1892,7 @@
         <v>28</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1906,7 +1906,7 @@
         <v>29</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1920,7 +1920,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1934,7 +1934,7 @@
         <v>31</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1948,7 +1948,7 @@
         <v>32</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2253,7 +2253,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>54</v>
+        <v>340</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>6</v>
@@ -2267,7 +2267,7 @@
         <v>5</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>6</v>
@@ -2290,10 +2290,10 @@
         <v>1</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>6</v>
@@ -2304,10 +2304,10 @@
         <v>2</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>6</v>
@@ -2318,10 +2318,10 @@
         <v>3</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>6</v>
@@ -2332,10 +2332,10 @@
         <v>4</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>6</v>
@@ -2346,10 +2346,10 @@
         <v>5</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>6</v>
@@ -2360,10 +2360,10 @@
         <v>6</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>6</v>
@@ -2374,10 +2374,10 @@
         <v>7</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>6</v>
@@ -2388,10 +2388,10 @@
         <v>8</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>6</v>
@@ -2402,10 +2402,10 @@
         <v>9</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>6</v>
@@ -2416,10 +2416,10 @@
         <v>10</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>6</v>
@@ -2430,10 +2430,10 @@
         <v>11</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>6</v>
@@ -2444,10 +2444,10 @@
         <v>12</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>6</v>
@@ -2458,10 +2458,10 @@
         <v>13</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>6</v>
@@ -2472,10 +2472,10 @@
         <v>14</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>6</v>
@@ -2486,10 +2486,10 @@
         <v>15</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>6</v>
@@ -2500,10 +2500,10 @@
         <v>16</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>6</v>
@@ -2514,10 +2514,10 @@
         <v>17</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>6</v>
@@ -2528,10 +2528,10 @@
         <v>18</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>6</v>
@@ -2542,10 +2542,10 @@
         <v>19</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>6</v>
@@ -2556,10 +2556,10 @@
         <v>20</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>6</v>
@@ -2570,10 +2570,10 @@
         <v>21</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>6</v>
@@ -2584,10 +2584,10 @@
         <v>22</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>6</v>
@@ -2598,10 +2598,10 @@
         <v>23</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>6</v>
@@ -2612,10 +2612,10 @@
         <v>24</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>6</v>
@@ -2626,10 +2626,10 @@
         <v>25</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>6</v>
@@ -2640,10 +2640,10 @@
         <v>26</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>6</v>
@@ -2654,10 +2654,10 @@
         <v>27</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>6</v>
@@ -2668,10 +2668,10 @@
         <v>28</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>6</v>
@@ -2682,10 +2682,10 @@
         <v>29</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>6</v>
@@ -2696,10 +2696,10 @@
         <v>30</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>6</v>
@@ -2710,10 +2710,10 @@
         <v>31</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>6</v>
@@ -2724,10 +2724,10 @@
         <v>32</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>6</v>
@@ -2738,10 +2738,10 @@
         <v>33</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>6</v>
@@ -2752,10 +2752,10 @@
         <v>34</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>6</v>
@@ -2766,10 +2766,10 @@
         <v>35</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>6</v>
@@ -2780,10 +2780,10 @@
         <v>36</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D91" s="7" t="s">
         <v>6</v>
@@ -2794,10 +2794,10 @@
         <v>37</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>6</v>
@@ -2808,10 +2808,10 @@
         <v>38</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D93" s="7" t="s">
         <v>6</v>
@@ -2822,10 +2822,10 @@
         <v>39</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>6</v>
@@ -2836,10 +2836,10 @@
         <v>40</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D95" s="7" t="s">
         <v>6</v>
@@ -2850,10 +2850,10 @@
         <v>41</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D96" s="7" t="s">
         <v>6</v>
@@ -2864,10 +2864,10 @@
         <v>42</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D97" s="7" t="s">
         <v>6</v>
@@ -2878,10 +2878,10 @@
         <v>43</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>6</v>
@@ -2892,10 +2892,10 @@
         <v>44</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>6</v>
@@ -2906,10 +2906,10 @@
         <v>45</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>6</v>
@@ -2920,10 +2920,10 @@
         <v>46</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>6</v>
@@ -2934,10 +2934,10 @@
         <v>47</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>6</v>
@@ -2948,10 +2948,10 @@
         <v>48</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>6</v>
@@ -2962,10 +2962,10 @@
         <v>49</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>6</v>
@@ -2976,10 +2976,10 @@
         <v>50</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>6</v>
@@ -3002,10 +3002,10 @@
         <v>1</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C108" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>6</v>
@@ -3016,10 +3016,10 @@
         <v>2</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D109" s="7" t="s">
         <v>6</v>
@@ -3030,10 +3030,10 @@
         <v>3</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>6</v>
@@ -3044,10 +3044,10 @@
         <v>4</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D111" s="7" t="s">
         <v>6</v>
@@ -3058,10 +3058,10 @@
         <v>5</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D112" s="7" t="s">
         <v>6</v>
@@ -3072,7 +3072,7 @@
         <v>6</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C113" s="6"/>
       <c r="D113" s="7"/>
@@ -3082,10 +3082,10 @@
         <v>7</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D114" s="7" t="s">
         <v>6</v>
@@ -3096,10 +3096,10 @@
         <v>8</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D115" s="7" t="s">
         <v>6</v>
@@ -3110,10 +3110,10 @@
         <v>9</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D116" s="7" t="s">
         <v>6</v>
@@ -3124,10 +3124,10 @@
         <v>10</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D117" s="7" t="s">
         <v>6</v>
@@ -3138,10 +3138,10 @@
         <v>11</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D118" s="7" t="s">
         <v>6</v>
@@ -3152,7 +3152,7 @@
         <v>12</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C119" s="6"/>
       <c r="D119" s="7"/>
@@ -3162,10 +3162,10 @@
         <v>13</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D120" s="7" t="s">
         <v>6</v>
@@ -3176,10 +3176,10 @@
         <v>14</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D121" s="7" t="s">
         <v>6</v>
@@ -3190,10 +3190,10 @@
         <v>15</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D122" s="7" t="s">
         <v>6</v>
@@ -3204,10 +3204,10 @@
         <v>16</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D123" s="7" t="s">
         <v>6</v>
@@ -3218,10 +3218,10 @@
         <v>17</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D124" s="7" t="s">
         <v>6</v>
@@ -3244,10 +3244,10 @@
         <v>1</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D127" s="7" t="s">
         <v>6</v>
@@ -3258,10 +3258,10 @@
         <v>2</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C128" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D128" s="7" t="s">
         <v>6</v>
@@ -3272,10 +3272,10 @@
         <v>3</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D129" s="7" t="s">
         <v>6</v>
@@ -3286,10 +3286,10 @@
         <v>4</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>6</v>
@@ -3300,7 +3300,7 @@
         <v>5</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C131" s="6"/>
       <c r="D131" s="7"/>
@@ -3310,10 +3310,10 @@
         <v>6</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C132" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D132" s="7" t="s">
         <v>6</v>
@@ -3324,10 +3324,10 @@
         <v>7</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D133" s="7" t="s">
         <v>6</v>
@@ -3338,10 +3338,10 @@
         <v>8</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D134" s="7" t="s">
         <v>6</v>
@@ -3352,10 +3352,10 @@
         <v>9</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D135" s="7" t="s">
         <v>6</v>
@@ -3366,10 +3366,10 @@
         <v>10</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D136" s="7" t="s">
         <v>6</v>
@@ -3380,7 +3380,7 @@
         <v>11</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C137" s="6"/>
       <c r="D137" s="7"/>
@@ -3390,10 +3390,10 @@
         <v>12</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D138" s="7" t="s">
         <v>6</v>
@@ -3404,10 +3404,10 @@
         <v>13</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D139" s="7" t="s">
         <v>6</v>
@@ -3418,10 +3418,10 @@
         <v>14</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D140" s="7" t="s">
         <v>6</v>
@@ -3432,10 +3432,10 @@
         <v>15</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D141" s="7" t="s">
         <v>6</v>
@@ -3458,10 +3458,10 @@
         <v>1</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D144" s="7" t="s">
         <v>6</v>
@@ -3472,10 +3472,10 @@
         <v>2</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D145" s="7" t="s">
         <v>6</v>
@@ -3486,10 +3486,10 @@
         <v>3</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D146" s="7" t="s">
         <v>6</v>
@@ -3500,10 +3500,10 @@
         <v>4</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D147" s="7" t="s">
         <v>6</v>
@@ -3514,10 +3514,10 @@
         <v>5</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D148" s="7" t="s">
         <v>6</v>
@@ -3528,7 +3528,7 @@
         <v>6</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C149" s="6"/>
       <c r="D149" s="7"/>
@@ -3538,10 +3538,10 @@
         <v>7</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C150" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D150" s="7" t="s">
         <v>6</v>
@@ -3552,10 +3552,10 @@
         <v>8</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D151" s="7" t="s">
         <v>6</v>
@@ -3566,10 +3566,10 @@
         <v>9</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C152" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D152" s="7" t="s">
         <v>6</v>
@@ -3580,10 +3580,10 @@
         <v>10</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D153" s="7" t="s">
         <v>6</v>
@@ -3594,10 +3594,10 @@
         <v>11</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D154" s="7" t="s">
         <v>6</v>
@@ -3608,7 +3608,7 @@
         <v>12</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C155" s="6"/>
       <c r="D155" s="7"/>
@@ -3618,10 +3618,10 @@
         <v>13</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C156" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D156" s="7" t="s">
         <v>6</v>
@@ -3632,10 +3632,10 @@
         <v>14</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D157" s="7" t="s">
         <v>6</v>
@@ -3646,10 +3646,10 @@
         <v>15</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D158" s="7" t="s">
         <v>6</v>
@@ -3660,10 +3660,10 @@
         <v>16</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C159" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D159" s="7" t="s">
         <v>6</v>
@@ -3686,10 +3686,10 @@
         <v>1</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D162" s="7" t="s">
         <v>6</v>
@@ -3700,10 +3700,10 @@
         <v>2</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C163" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D163" s="7" t="s">
         <v>6</v>
@@ -3714,10 +3714,10 @@
         <v>3</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C164" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D164" s="7" t="s">
         <v>6</v>
@@ -3728,10 +3728,10 @@
         <v>4</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C165" s="9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D165" s="7" t="s">
         <v>6</v>
@@ -3742,7 +3742,7 @@
         <v>5</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C166" s="6"/>
       <c r="D166" s="7"/>
@@ -3752,10 +3752,10 @@
         <v>6</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C167" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D167" s="7" t="s">
         <v>6</v>
@@ -3766,10 +3766,10 @@
         <v>7</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D168" s="7" t="s">
         <v>6</v>
@@ -3780,10 +3780,10 @@
         <v>8</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D169" s="7" t="s">
         <v>6</v>
@@ -3794,10 +3794,10 @@
         <v>9</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D170" s="7" t="s">
         <v>6</v>
@@ -3808,10 +3808,10 @@
         <v>10</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D171" s="7" t="s">
         <v>6</v>
@@ -3822,7 +3822,7 @@
         <v>11</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C172" s="6"/>
       <c r="D172" s="7"/>
@@ -3832,10 +3832,10 @@
         <v>12</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D173" s="7" t="s">
         <v>6</v>
@@ -3846,10 +3846,10 @@
         <v>13</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C174" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D174" s="7" t="s">
         <v>6</v>
@@ -3860,10 +3860,10 @@
         <v>14</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D175" s="7" t="s">
         <v>6</v>
@@ -3874,10 +3874,10 @@
         <v>15</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D176" s="7" t="s">
         <v>6</v>
@@ -3888,10 +3888,10 @@
         <v>16</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C177" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D177" s="7" t="s">
         <v>6</v>
@@ -3902,10 +3902,10 @@
         <v>17</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D178" s="7" t="s">
         <v>6</v>
@@ -3916,10 +3916,10 @@
         <v>18</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C179" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D179" s="7" t="s">
         <v>6</v>
@@ -3942,10 +3942,10 @@
         <v>1</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C182" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D182" s="7" t="s">
         <v>6</v>
@@ -3956,10 +3956,10 @@
         <v>2</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C183" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D183" s="7" t="s">
         <v>6</v>
@@ -3970,10 +3970,10 @@
         <v>3</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D184" s="7" t="s">
         <v>6</v>
@@ -3984,10 +3984,10 @@
         <v>4</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C185" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D185" s="7" t="s">
         <v>6</v>
@@ -3998,10 +3998,10 @@
         <v>5</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C186" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D186" s="7" t="s">
         <v>6</v>
@@ -4012,10 +4012,10 @@
         <v>6</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C187" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D187" s="7" t="s">
         <v>6</v>
@@ -4026,10 +4026,10 @@
         <v>7</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C188" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D188" s="7" t="s">
         <v>6</v>
@@ -4040,7 +4040,7 @@
         <v>8</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C189" s="6"/>
       <c r="D189" s="7"/>
@@ -4050,10 +4050,10 @@
         <v>9</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C190" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D190" s="7" t="s">
         <v>6</v>
@@ -4064,10 +4064,10 @@
         <v>10</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C191" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D191" s="7" t="s">
         <v>6</v>
@@ -4078,10 +4078,10 @@
         <v>11</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C192" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D192" s="7" t="s">
         <v>6</v>
@@ -4092,10 +4092,10 @@
         <v>12</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C193" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D193" s="7" t="s">
         <v>6</v>
@@ -4106,10 +4106,10 @@
         <v>13</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C194" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D194" s="7" t="s">
         <v>6</v>
@@ -4120,10 +4120,10 @@
         <v>14</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D195" s="7" t="s">
         <v>6</v>
@@ -4134,10 +4134,10 @@
         <v>15</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C196" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D196" s="7" t="s">
         <v>6</v>
@@ -4148,10 +4148,10 @@
         <v>16</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C197" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D197" s="7" t="s">
         <v>6</v>
@@ -4162,10 +4162,10 @@
         <v>17</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C198" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D198" s="7" t="s">
         <v>6</v>
@@ -4176,7 +4176,7 @@
         <v>18</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C199" s="6"/>
       <c r="D199" s="7"/>
@@ -4186,10 +4186,10 @@
         <v>19</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C200" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D200" s="7" t="s">
         <v>6</v>
@@ -4200,10 +4200,10 @@
         <v>20</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D201" s="7" t="s">
         <v>6</v>
@@ -4214,10 +4214,10 @@
         <v>21</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C202" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D202" s="7" t="s">
         <v>6</v>
@@ -4228,10 +4228,10 @@
         <v>22</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C203" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D203" s="7" t="s">
         <v>6</v>
@@ -4242,10 +4242,10 @@
         <v>23</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D204" s="7" t="s">
         <v>6</v>
@@ -4256,10 +4256,10 @@
         <v>24</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D205" s="7" t="s">
         <v>6</v>
@@ -4282,10 +4282,10 @@
         <v>1</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D208" s="7" t="s">
         <v>6</v>
@@ -4308,10 +4308,10 @@
         <v>1</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C211" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D211" s="7" t="s">
         <v>6</v>
@@ -4322,10 +4322,10 @@
         <v>2</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C212" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D212" s="7" t="s">
         <v>6</v>
@@ -4336,10 +4336,10 @@
         <v>3</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C213" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D213" s="7" t="s">
         <v>6</v>
@@ -4350,10 +4350,10 @@
         <v>4</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D214" s="7" t="s">
         <v>6</v>
@@ -4364,10 +4364,10 @@
         <v>5</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C215" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D215" s="7" t="s">
         <v>6</v>
@@ -4378,7 +4378,7 @@
         <v>6</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C216" s="6"/>
       <c r="D216" s="7"/>
@@ -4388,10 +4388,10 @@
         <v>7</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C217" s="10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D217" s="7" t="s">
         <v>6</v>
@@ -4402,10 +4402,10 @@
         <v>8</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D218" s="7" t="s">
         <v>6</v>
@@ -4416,10 +4416,10 @@
         <v>9</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C219" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D219" s="7" t="s">
         <v>6</v>
@@ -4430,10 +4430,10 @@
         <v>10</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C220" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D220" s="7" t="s">
         <v>6</v>
@@ -4456,10 +4456,10 @@
         <v>1</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C223" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D223" s="7" t="s">
         <v>6</v>
@@ -4470,7 +4470,7 @@
         <v>2</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C224" s="11"/>
       <c r="D224" s="7" t="s">
@@ -4482,10 +4482,10 @@
         <v>3</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C225" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D225" s="7" t="s">
         <v>6</v>
@@ -4496,10 +4496,10 @@
         <v>4</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C226" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D226" s="7" t="s">
         <v>6</v>
@@ -4510,7 +4510,7 @@
         <v>5</v>
       </c>
       <c r="B227" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C227" s="6"/>
       <c r="D227" s="7"/>
@@ -4520,10 +4520,10 @@
         <v>6</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C228" s="10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D228" s="7" t="s">
         <v>6</v>
@@ -4534,7 +4534,7 @@
         <v>7</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C229" s="11"/>
       <c r="D229" s="7" t="s">
@@ -4546,10 +4546,10 @@
         <v>8</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C230" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D230" s="7" t="s">
         <v>6</v>
@@ -4560,10 +4560,10 @@
         <v>9</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C231" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D231" s="7" t="s">
         <v>6</v>
@@ -4574,10 +4574,10 @@
         <v>10</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C232" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D232" s="7" t="s">
         <v>6</v>
@@ -4588,10 +4588,10 @@
         <v>11</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D233" s="7" t="s">
         <v>6</v>
@@ -4602,7 +4602,7 @@
         <v>12</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C234" s="6"/>
       <c r="D234" s="7"/>
@@ -4612,10 +4612,10 @@
         <v>13</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C235" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D235" s="7" t="s">
         <v>6</v>
@@ -4626,7 +4626,7 @@
         <v>14</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C236" s="11"/>
       <c r="D236" s="7" t="s">
@@ -4638,10 +4638,10 @@
         <v>15</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C237" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D237" s="7" t="s">
         <v>6</v>
@@ -4652,10 +4652,10 @@
         <v>16</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C238" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D238" s="7" t="s">
         <v>6</v>
@@ -4666,10 +4666,10 @@
         <v>17</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C239" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D239" s="7" t="s">
         <v>6</v>
@@ -4680,10 +4680,10 @@
         <v>18</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C240" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D240" s="7" t="s">
         <v>6</v>
@@ -4694,7 +4694,7 @@
         <v>19</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C241" s="6"/>
       <c r="D241" s="7"/>
@@ -4704,10 +4704,10 @@
         <v>20</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C242" s="10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D242" s="7" t="s">
         <v>6</v>
@@ -4718,7 +4718,7 @@
         <v>21</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C243" s="11"/>
       <c r="D243" s="7" t="s">
@@ -4730,10 +4730,10 @@
         <v>22</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C244" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D244" s="7" t="s">
         <v>6</v>
@@ -4744,10 +4744,10 @@
         <v>23</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C245" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D245" s="7" t="s">
         <v>6</v>
@@ -4770,10 +4770,10 @@
         <v>1</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D248" s="7" t="s">
         <v>6</v>
@@ -4784,10 +4784,10 @@
         <v>2</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D249" s="7" t="s">
         <v>6</v>
@@ -4798,10 +4798,10 @@
         <v>3</v>
       </c>
       <c r="B250" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C250" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="C250" s="9" t="s">
-        <v>214</v>
       </c>
       <c r="D250" s="7" t="s">
         <v>6</v>
@@ -4812,10 +4812,10 @@
         <v>4</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D251" s="7" t="s">
         <v>6</v>
@@ -4826,10 +4826,10 @@
         <v>5</v>
       </c>
       <c r="B252" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D252" s="7" t="s">
         <v>6</v>
@@ -4840,10 +4840,10 @@
         <v>6</v>
       </c>
       <c r="B253" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C253" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D253" s="7" t="s">
         <v>6</v>
@@ -4854,10 +4854,10 @@
         <v>7</v>
       </c>
       <c r="B254" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D254" s="7" t="s">
         <v>6</v>
@@ -4868,10 +4868,10 @@
         <v>8</v>
       </c>
       <c r="B255" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D255" s="7" t="s">
         <v>6</v>
@@ -4882,10 +4882,10 @@
         <v>9</v>
       </c>
       <c r="B256" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D256" s="7" t="s">
         <v>6</v>
@@ -4896,7 +4896,7 @@
         <v>10</v>
       </c>
       <c r="B257" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C257" s="6"/>
       <c r="D257" s="7"/>
@@ -4906,10 +4906,10 @@
         <v>11</v>
       </c>
       <c r="B258" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C258" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D258" s="7" t="s">
         <v>6</v>
@@ -4920,10 +4920,10 @@
         <v>12</v>
       </c>
       <c r="B259" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D259" s="7" t="s">
         <v>6</v>
@@ -4934,10 +4934,10 @@
         <v>13</v>
       </c>
       <c r="B260" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D260" s="7" t="s">
         <v>6</v>
@@ -4948,10 +4948,10 @@
         <v>14</v>
       </c>
       <c r="B261" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D261" s="7" t="s">
         <v>6</v>
@@ -4962,10 +4962,10 @@
         <v>15</v>
       </c>
       <c r="B262" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C262" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D262" s="7" t="s">
         <v>6</v>
@@ -4976,10 +4976,10 @@
         <v>16</v>
       </c>
       <c r="B263" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C263" s="9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D263" s="7" t="s">
         <v>6</v>
@@ -4990,10 +4990,10 @@
         <v>17</v>
       </c>
       <c r="B264" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D264" s="7" t="s">
         <v>6</v>
@@ -5004,10 +5004,10 @@
         <v>18</v>
       </c>
       <c r="B265" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C265" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D265" s="7" t="s">
         <v>6</v>
@@ -5018,10 +5018,10 @@
         <v>19</v>
       </c>
       <c r="B266" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C266" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D266" s="7" t="s">
         <v>6</v>
@@ -5032,10 +5032,10 @@
         <v>20</v>
       </c>
       <c r="B267" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C267" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D267" s="7" t="s">
         <v>6</v>
@@ -5046,7 +5046,7 @@
         <v>21</v>
       </c>
       <c r="B268" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C268" s="6"/>
       <c r="D268" s="7"/>
@@ -5056,10 +5056,10 @@
         <v>22</v>
       </c>
       <c r="B269" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C269" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D269" s="7" t="s">
         <v>6</v>
@@ -5070,10 +5070,10 @@
         <v>23</v>
       </c>
       <c r="B270" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D270" s="7" t="s">
         <v>6</v>
@@ -5084,10 +5084,10 @@
         <v>24</v>
       </c>
       <c r="B271" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D271" s="7" t="s">
         <v>6</v>
@@ -5098,10 +5098,10 @@
         <v>25</v>
       </c>
       <c r="B272" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D272" s="7" t="s">
         <v>6</v>
@@ -5112,10 +5112,10 @@
         <v>26</v>
       </c>
       <c r="B273" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C273" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D273" s="7" t="s">
         <v>6</v>
@@ -5126,10 +5126,10 @@
         <v>27</v>
       </c>
       <c r="B274" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C274" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D274" s="7" t="s">
         <v>6</v>
@@ -5152,10 +5152,10 @@
         <v>1</v>
       </c>
       <c r="B277" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D277" s="7" t="s">
         <v>6</v>
@@ -5166,10 +5166,10 @@
         <v>2</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D278" s="7" t="s">
         <v>6</v>
@@ -5180,10 +5180,10 @@
         <v>3</v>
       </c>
       <c r="B279" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C279" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D279" s="7" t="s">
         <v>6</v>
@@ -5194,10 +5194,10 @@
         <v>4</v>
       </c>
       <c r="B280" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C280" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D280" s="7" t="s">
         <v>6</v>
@@ -5208,10 +5208,10 @@
         <v>5</v>
       </c>
       <c r="B281" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D281" s="7" t="s">
         <v>6</v>
@@ -5222,10 +5222,10 @@
         <v>6</v>
       </c>
       <c r="B282" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D282" s="7" t="s">
         <v>6</v>
@@ -5248,10 +5248,10 @@
         <v>1</v>
       </c>
       <c r="B285" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D285" s="7" t="s">
         <v>6</v>
@@ -5262,10 +5262,10 @@
         <v>2</v>
       </c>
       <c r="B286" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C286" s="9" t="s">
         <v>241</v>
-      </c>
-      <c r="C286" s="9" t="s">
-        <v>243</v>
       </c>
       <c r="D286" s="7" t="s">
         <v>6</v>
@@ -5276,10 +5276,10 @@
         <v>3</v>
       </c>
       <c r="B287" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D287" s="7" t="s">
         <v>6</v>
@@ -5290,10 +5290,10 @@
         <v>4</v>
       </c>
       <c r="B288" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D288" s="7" t="s">
         <v>6</v>
@@ -5304,10 +5304,10 @@
         <v>5</v>
       </c>
       <c r="B289" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D289" s="7" t="s">
         <v>6</v>
@@ -5318,10 +5318,10 @@
         <v>6</v>
       </c>
       <c r="B290" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D290" s="7" t="s">
         <v>6</v>
@@ -5332,10 +5332,10 @@
         <v>7</v>
       </c>
       <c r="B291" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D291" s="7" t="s">
         <v>6</v>
@@ -5346,10 +5346,10 @@
         <v>8</v>
       </c>
       <c r="B292" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D292" s="7" t="s">
         <v>6</v>
@@ -5372,10 +5372,10 @@
         <v>1</v>
       </c>
       <c r="B295" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C295" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D295" s="7" t="s">
         <v>6</v>
@@ -5386,10 +5386,10 @@
         <v>2</v>
       </c>
       <c r="B296" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D296" s="7" t="s">
         <v>6</v>
@@ -5400,10 +5400,10 @@
         <v>3</v>
       </c>
       <c r="B297" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D297" s="7" t="s">
         <v>6</v>
@@ -5414,10 +5414,10 @@
         <v>4</v>
       </c>
       <c r="B298" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C298" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D298" s="7" t="s">
         <v>6</v>
@@ -5428,10 +5428,10 @@
         <v>5</v>
       </c>
       <c r="B299" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C299" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D299" s="7" t="s">
         <v>6</v>
@@ -5442,10 +5442,10 @@
         <v>6</v>
       </c>
       <c r="B300" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C300" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D300" s="7" t="s">
         <v>6</v>
@@ -5456,10 +5456,10 @@
         <v>7</v>
       </c>
       <c r="B301" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C301" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D301" s="7" t="s">
         <v>6</v>
@@ -5470,10 +5470,10 @@
         <v>8</v>
       </c>
       <c r="B302" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C302" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D302" s="7" t="s">
         <v>6</v>
@@ -5484,10 +5484,10 @@
         <v>9</v>
       </c>
       <c r="B303" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C303" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D303" s="7" t="s">
         <v>6</v>
@@ -5498,10 +5498,10 @@
         <v>10</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C304" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D304" s="7" t="s">
         <v>6</v>
@@ -5512,10 +5512,10 @@
         <v>11</v>
       </c>
       <c r="B305" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C305" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D305" s="7" t="s">
         <v>6</v>
@@ -5526,10 +5526,10 @@
         <v>12</v>
       </c>
       <c r="B306" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C306" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D306" s="7" t="s">
         <v>6</v>
@@ -5540,10 +5540,10 @@
         <v>13</v>
       </c>
       <c r="B307" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C307" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D307" s="7" t="s">
         <v>6</v>
@@ -5554,10 +5554,10 @@
         <v>14</v>
       </c>
       <c r="B308" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C308" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D308" s="7" t="s">
         <v>6</v>
@@ -5568,10 +5568,10 @@
         <v>15</v>
       </c>
       <c r="B309" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C309" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D309" s="7" t="s">
         <v>6</v>
@@ -5582,10 +5582,10 @@
         <v>16</v>
       </c>
       <c r="B310" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C310" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D310" s="7" t="s">
         <v>6</v>
@@ -5596,7 +5596,7 @@
         <v>17</v>
       </c>
       <c r="B311" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C311" s="6"/>
       <c r="D311" s="7"/>
@@ -5606,10 +5606,10 @@
         <v>18</v>
       </c>
       <c r="B312" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C312" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D312" s="7" t="s">
         <v>6</v>
@@ -5620,10 +5620,10 @@
         <v>19</v>
       </c>
       <c r="B313" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C313" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D313" s="7" t="s">
         <v>6</v>
@@ -5634,10 +5634,10 @@
         <v>20</v>
       </c>
       <c r="B314" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C314" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D314" s="7" t="s">
         <v>6</v>
@@ -5648,10 +5648,10 @@
         <v>21</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C315" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D315" s="7" t="s">
         <v>6</v>
@@ -5662,10 +5662,10 @@
         <v>22</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C316" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D316" s="7" t="s">
         <v>6</v>
@@ -5676,10 +5676,10 @@
         <v>23</v>
       </c>
       <c r="B317" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C317" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D317" s="7" t="s">
         <v>6</v>
@@ -5690,10 +5690,10 @@
         <v>24</v>
       </c>
       <c r="B318" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C318" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D318" s="7" t="s">
         <v>6</v>
@@ -5704,10 +5704,10 @@
         <v>25</v>
       </c>
       <c r="B319" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C319" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D319" s="7" t="s">
         <v>6</v>
@@ -5718,10 +5718,10 @@
         <v>26</v>
       </c>
       <c r="B320" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C320" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D320" s="7" t="s">
         <v>6</v>
@@ -5732,10 +5732,10 @@
         <v>27</v>
       </c>
       <c r="B321" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C321" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D321" s="7" t="s">
         <v>6</v>
@@ -5746,10 +5746,10 @@
         <v>28</v>
       </c>
       <c r="B322" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C322" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D322" s="7" t="s">
         <v>6</v>
@@ -5760,7 +5760,7 @@
         <v>29</v>
       </c>
       <c r="B323" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C323" s="6"/>
       <c r="D323" s="7"/>
@@ -5770,10 +5770,10 @@
         <v>30</v>
       </c>
       <c r="B324" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C324" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D324" s="7" t="s">
         <v>6</v>
@@ -5784,10 +5784,10 @@
         <v>31</v>
       </c>
       <c r="B325" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C325" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D325" s="7" t="s">
         <v>6</v>
@@ -5798,10 +5798,10 @@
         <v>32</v>
       </c>
       <c r="B326" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C326" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D326" s="7" t="s">
         <v>6</v>
@@ -5812,10 +5812,10 @@
         <v>33</v>
       </c>
       <c r="B327" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C327" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D327" s="7" t="s">
         <v>6</v>
@@ -5826,10 +5826,10 @@
         <v>34</v>
       </c>
       <c r="B328" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C328" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D328" s="7" t="s">
         <v>6</v>
@@ -5840,10 +5840,10 @@
         <v>35</v>
       </c>
       <c r="B329" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C329" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D329" s="7" t="s">
         <v>6</v>
@@ -5854,10 +5854,10 @@
         <v>36</v>
       </c>
       <c r="B330" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C330" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D330" s="7" t="s">
         <v>6</v>
@@ -5868,10 +5868,10 @@
         <v>37</v>
       </c>
       <c r="B331" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C331" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D331" s="7" t="s">
         <v>6</v>
@@ -5882,10 +5882,10 @@
         <v>38</v>
       </c>
       <c r="B332" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C332" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D332" s="7" t="s">
         <v>6</v>
@@ -5896,10 +5896,10 @@
         <v>39</v>
       </c>
       <c r="B333" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C333" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D333" s="7" t="s">
         <v>6</v>
@@ -5910,10 +5910,10 @@
         <v>40</v>
       </c>
       <c r="B334" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C334" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D334" s="7" t="s">
         <v>6</v>
@@ -5936,10 +5936,10 @@
         <v>1</v>
       </c>
       <c r="B337" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C337" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D337" s="7" t="s">
         <v>6</v>
@@ -5950,10 +5950,10 @@
         <v>2</v>
       </c>
       <c r="B338" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C338" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D338" s="7" t="s">
         <v>6</v>
@@ -5964,10 +5964,10 @@
         <v>3</v>
       </c>
       <c r="B339" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C339" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D339" s="7" t="s">
         <v>6</v>
@@ -5978,10 +5978,10 @@
         <v>4</v>
       </c>
       <c r="B340" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C340" s="9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D340" s="7" t="s">
         <v>6</v>
@@ -5992,7 +5992,7 @@
         <v>5</v>
       </c>
       <c r="B341" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C341" s="6"/>
       <c r="D341" s="7"/>
@@ -6002,10 +6002,10 @@
         <v>6</v>
       </c>
       <c r="B342" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C342" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D342" s="7" t="s">
         <v>6</v>
@@ -6016,10 +6016,10 @@
         <v>7</v>
       </c>
       <c r="B343" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C343" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D343" s="7" t="s">
         <v>6</v>
@@ -6030,10 +6030,10 @@
         <v>8</v>
       </c>
       <c r="B344" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C344" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D344" s="7" t="s">
         <v>6</v>
@@ -6044,10 +6044,10 @@
         <v>9</v>
       </c>
       <c r="B345" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C345" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D345" s="7" t="s">
         <v>6</v>
@@ -6058,7 +6058,7 @@
         <v>10</v>
       </c>
       <c r="B346" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C346" s="6"/>
       <c r="D346" s="7"/>
@@ -6068,10 +6068,10 @@
         <v>11</v>
       </c>
       <c r="B347" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C347" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D347" s="7" t="s">
         <v>6</v>
@@ -6082,10 +6082,10 @@
         <v>12</v>
       </c>
       <c r="B348" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C348" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D348" s="7" t="s">
         <v>6</v>
@@ -6096,10 +6096,10 @@
         <v>13</v>
       </c>
       <c r="B349" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C349" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D349" s="7" t="s">
         <v>6</v>
@@ -6110,10 +6110,10 @@
         <v>14</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C350" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D350" s="7" t="s">
         <v>6</v>
@@ -6124,10 +6124,10 @@
         <v>15</v>
       </c>
       <c r="B351" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C351" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D351" s="7" t="s">
         <v>6</v>
@@ -6150,10 +6150,10 @@
         <v>1</v>
       </c>
       <c r="B354" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C354" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D354" s="7" t="s">
         <v>6</v>
@@ -6164,10 +6164,10 @@
         <v>2</v>
       </c>
       <c r="B355" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C355" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D355" s="7" t="s">
         <v>6</v>
@@ -6178,10 +6178,10 @@
         <v>3</v>
       </c>
       <c r="B356" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C356" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D356" s="7" t="s">
         <v>6</v>
@@ -6192,10 +6192,10 @@
         <v>4</v>
       </c>
       <c r="B357" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C357" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D357" s="7" t="s">
         <v>6</v>
@@ -6206,10 +6206,10 @@
         <v>5</v>
       </c>
       <c r="B358" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C358" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D358" s="7" t="s">
         <v>6</v>
@@ -6220,10 +6220,10 @@
         <v>6</v>
       </c>
       <c r="B359" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C359" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D359" s="7" t="s">
         <v>6</v>
@@ -6246,10 +6246,10 @@
         <v>1</v>
       </c>
       <c r="B362" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C362" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D362" s="7" t="s">
         <v>6</v>
@@ -6260,10 +6260,10 @@
         <v>2</v>
       </c>
       <c r="B363" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C363" s="9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D363" s="7" t="s">
         <v>6</v>
@@ -6274,10 +6274,10 @@
         <v>3</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C364" s="9" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D364" s="7" t="s">
         <v>6</v>
@@ -6288,10 +6288,10 @@
         <v>4</v>
       </c>
       <c r="B365" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C365" s="9" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D365" s="7" t="s">
         <v>6</v>
@@ -6302,10 +6302,10 @@
         <v>5</v>
       </c>
       <c r="B366" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C366" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D366" s="7" t="s">
         <v>6</v>
@@ -6316,10 +6316,10 @@
         <v>6</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C367" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D367" s="7" t="s">
         <v>6</v>
@@ -6330,10 +6330,10 @@
         <v>7</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C368" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D368" s="7" t="s">
         <v>6</v>
@@ -6344,10 +6344,10 @@
         <v>8</v>
       </c>
       <c r="B369" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C369" s="9" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D369" s="7" t="s">
         <v>6</v>
@@ -6358,10 +6358,10 @@
         <v>9</v>
       </c>
       <c r="B370" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C370" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D370" s="7" t="s">
         <v>6</v>
@@ -6372,10 +6372,10 @@
         <v>10</v>
       </c>
       <c r="B371" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C371" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D371" s="7" t="s">
         <v>6</v>
@@ -6386,10 +6386,10 @@
         <v>11</v>
       </c>
       <c r="B372" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C372" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D372" s="7" t="s">
         <v>6</v>
@@ -6400,10 +6400,10 @@
         <v>12</v>
       </c>
       <c r="B373" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C373" s="9" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D373" s="7" t="s">
         <v>6</v>
@@ -6426,10 +6426,10 @@
         <v>1</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C376" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D376" s="7" t="s">
         <v>6</v>
@@ -6440,10 +6440,10 @@
         <v>2</v>
       </c>
       <c r="B377" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C377" s="9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D377" s="7" t="s">
         <v>6</v>
@@ -6454,10 +6454,10 @@
         <v>3</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C378" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D378" s="7" t="s">
         <v>6</v>
@@ -6468,10 +6468,10 @@
         <v>4</v>
       </c>
       <c r="B379" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C379" s="9" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D379" s="7" t="s">
         <v>6</v>
@@ -6482,10 +6482,10 @@
         <v>5</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C380" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D380" s="7" t="s">
         <v>6</v>
@@ -6496,10 +6496,10 @@
         <v>6</v>
       </c>
       <c r="B381" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C381" s="9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D381" s="7" t="s">
         <v>6</v>
@@ -6510,10 +6510,10 @@
         <v>7</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C382" s="9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D382" s="7" t="s">
         <v>6</v>
@@ -6524,10 +6524,10 @@
         <v>8</v>
       </c>
       <c r="B383" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C383" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D383" s="7" t="s">
         <v>6</v>
@@ -6538,10 +6538,10 @@
         <v>9</v>
       </c>
       <c r="B384" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C384" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D384" s="7" t="s">
         <v>6</v>
@@ -6552,10 +6552,10 @@
         <v>10</v>
       </c>
       <c r="B385" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C385" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D385" s="7" t="s">
         <v>6</v>
@@ -6566,10 +6566,10 @@
         <v>11</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C386" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D386" s="7" t="s">
         <v>6</v>
@@ -6580,10 +6580,10 @@
         <v>12</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C387" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D387" s="7" t="s">
         <v>6</v>
@@ -6594,10 +6594,10 @@
         <v>13</v>
       </c>
       <c r="B388" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C388" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D388" s="7" t="s">
         <v>6</v>
@@ -6608,10 +6608,10 @@
         <v>14</v>
       </c>
       <c r="B389" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C389" s="9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D389" s="7" t="s">
         <v>6</v>
@@ -6622,10 +6622,10 @@
         <v>15</v>
       </c>
       <c r="B390" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C390" s="9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D390" s="7" t="s">
         <v>6</v>
@@ -6646,10 +6646,10 @@
         <v>1</v>
       </c>
       <c r="B393" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C393" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D393" s="7" t="s">
         <v>6</v>
@@ -6660,10 +6660,10 @@
         <v>2</v>
       </c>
       <c r="B394" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C394" s="9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D394" s="7" t="s">
         <v>6</v>
@@ -6674,10 +6674,10 @@
         <v>3</v>
       </c>
       <c r="B395" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C395" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D395" s="7" t="s">
         <v>6</v>
@@ -6688,10 +6688,10 @@
         <v>4</v>
       </c>
       <c r="B396" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C396" s="9" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D396" s="7" t="s">
         <v>6</v>
@@ -6702,10 +6702,10 @@
         <v>5</v>
       </c>
       <c r="B397" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C397" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D397" s="7" t="s">
         <v>6</v>
@@ -6716,10 +6716,10 @@
         <v>6</v>
       </c>
       <c r="B398" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C398" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D398" s="7" t="s">
         <v>6</v>
@@ -6748,311 +6748,311 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="https://codeforces.com/problemset/problem/282/A" xr:uid="{7AD4378C-C6E3-4919-AB2D-1E79EA4AE89C}"/>
-    <hyperlink ref="C5" r:id="rId2" display="https://codeforces.com/contest/514/problem/A" xr:uid="{CEA0875B-88E2-45C1-9A71-CF088225271A}"/>
-    <hyperlink ref="C6" r:id="rId3" display="https://codeforces.com/problemset/problem/263/A" xr:uid="{2F2F77A2-1448-4700-846F-88BEA70E2D50}"/>
-    <hyperlink ref="C7" r:id="rId4" display="https://codeforces.com/problemset/problem/151/A" xr:uid="{533530EF-4093-4BA3-A2DD-E140C2088301}"/>
-    <hyperlink ref="C8" r:id="rId5" display="https://codeforces.com/problemset/problem/723/A" xr:uid="{50D3AB2C-AD9E-4FE0-A569-F740E153FFEE}"/>
-    <hyperlink ref="C9" r:id="rId6" display="https://codeforces.com/problemset/problem/1352/A" xr:uid="{F533AD00-4C0D-44B5-BF73-F3295AEEC9F5}"/>
-    <hyperlink ref="C10" r:id="rId7" display="https://codeforces.com/problemset/problem/510/A" xr:uid="{ABD9DC67-9903-400B-B55A-550FB3B3F4E1}"/>
-    <hyperlink ref="C11" r:id="rId8" display="https://codeforces.com/problemset/problem/785/A" xr:uid="{3FC19171-6ACB-495A-B1A8-E084699236B8}"/>
-    <hyperlink ref="C12" r:id="rId9" display="https://codeforces.com/problemset/problem/144/A" xr:uid="{21B96339-A0F1-480F-BEE1-00F73846DF55}"/>
-    <hyperlink ref="C13" r:id="rId10" display="https://codeforces.com/problemset/problem/1030/A" xr:uid="{23F44901-AF47-491D-A29A-69BCA7A6E040}"/>
-    <hyperlink ref="C14" r:id="rId11" display="https://codeforces.com/problemset/problem/136/A" xr:uid="{412D3794-2E50-44C6-8C93-E72FF6F1F68B}"/>
-    <hyperlink ref="C15" r:id="rId12" display="https://codeforces.com/problemset/problem/110/A" xr:uid="{57D7F86C-86B6-46FB-8859-51209D7FB1DA}"/>
-    <hyperlink ref="C16" r:id="rId13" display="https://codeforces.com/problemset/problem/116/A" xr:uid="{82280229-BCE5-4121-8E29-8E79656D98FF}"/>
-    <hyperlink ref="C17" r:id="rId14" display="https://codeforces.com/problemset/problem/977/A" xr:uid="{C58D39AF-0D61-4925-ADAC-B9A3C881CED5}"/>
-    <hyperlink ref="C18" r:id="rId15" display="https://codeforces.com/problemset/problem/546/A" xr:uid="{CBAEC032-DE0E-44F7-88D0-392BC2082D0B}"/>
-    <hyperlink ref="C19" r:id="rId16" display="https://codeforces.com/problemset/problem/791/A" xr:uid="{741F15CC-C2FD-4522-A332-026966058829}"/>
-    <hyperlink ref="C20" r:id="rId17" display="https://codeforces.com/problemset/problem/236/A" xr:uid="{92C81E6D-9E22-4119-AE35-44645C0D4559}"/>
-    <hyperlink ref="C21" r:id="rId18" display="https://codeforces.com/problemset/problem/281/A" xr:uid="{B649CB97-4BC2-4B09-A405-A92914E7BEE5}"/>
-    <hyperlink ref="C22" r:id="rId19" display="https://codeforces.com/problemset/problem/339/A" xr:uid="{0BB10978-FF6E-4841-9FBA-1C8F61DB200C}"/>
-    <hyperlink ref="C23" r:id="rId20" display="https://codeforces.com/problemset/problem/1368/A" xr:uid="{C38A1BD2-557E-4294-9C66-89003B4582EB}"/>
-    <hyperlink ref="C24" r:id="rId21" display="https://codeforces.com/problemset/problem/702/A" xr:uid="{5138572A-1A8A-4802-9CC9-9F09442F9D8D}"/>
-    <hyperlink ref="C25" r:id="rId22" display="https://codeforces.com/problemset/problem/1097/A" xr:uid="{72DBB92F-59A5-4D57-977F-78A760A879EC}"/>
-    <hyperlink ref="C26" r:id="rId23" display="https://codeforces.com/problemset/problem/492/A" xr:uid="{1C40A7AC-E454-4F49-A6D5-9E0526DF301A}"/>
-    <hyperlink ref="C27" r:id="rId24" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{EC6F9A74-8DCB-4075-A70D-F176385BAEAA}"/>
-    <hyperlink ref="C28" r:id="rId25" xr:uid="{7FA95D5D-D2D4-4485-95B8-3FB9DB984458}"/>
-    <hyperlink ref="C29" r:id="rId26" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{D34F22C4-83E3-47E7-BB16-78AF65773263}"/>
-    <hyperlink ref="C30" r:id="rId27" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{9E927AFA-8971-485C-BB32-775F2E25E8A9}"/>
-    <hyperlink ref="C31" r:id="rId28" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{D54316AA-F172-4382-B4BD-A45A7AAB9719}"/>
-    <hyperlink ref="C32" r:id="rId29" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{FB76318D-0FA6-4997-9291-9E5F8A30CD6B}"/>
-    <hyperlink ref="C33" r:id="rId30" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{2D2562E2-3649-429B-A34B-AB25B02329F1}"/>
-    <hyperlink ref="C34" r:id="rId31" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{FA75EBC9-C923-46B0-A46F-29307947C3D5}"/>
-    <hyperlink ref="C35" r:id="rId32" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{FD65AB9F-9FCF-4743-B03B-84BC789CB6F9}"/>
-    <hyperlink ref="C36" r:id="rId33" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{1AEA8404-C474-40D1-97DD-8D893B64F0B7}"/>
-    <hyperlink ref="C37" r:id="rId34" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{921646B8-ECD6-4B55-8E42-735C354A5243}"/>
-    <hyperlink ref="C38" r:id="rId35" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{8800A0EC-B145-4766-A02C-FA148D086B9A}"/>
-    <hyperlink ref="C39" r:id="rId36" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{E077F1DE-E7C3-481B-BA88-71BA2D07C7F1}"/>
-    <hyperlink ref="C40" r:id="rId37" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{04182062-C9D9-4AB2-AE3B-9ED317C1AE00}"/>
-    <hyperlink ref="C41" r:id="rId38" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{DF29D721-1927-49CD-83DA-671230898BAA}"/>
-    <hyperlink ref="C42" r:id="rId39" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{27B7B8D5-E56B-4398-8068-87FD298F2F6D}"/>
-    <hyperlink ref="C43" r:id="rId40" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{1AEFB517-359C-4D53-B343-64B82A17D82A}"/>
-    <hyperlink ref="C44" r:id="rId41" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{FA85FAE1-F47A-4357-8E3D-DF087FE752AE}"/>
-    <hyperlink ref="C45" r:id="rId42" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{CB517C4C-8C6B-4F97-9B3B-5C76EC239F78}"/>
-    <hyperlink ref="C46" r:id="rId43" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{BB4040FE-59AB-44A4-87B5-733EBAF8DCA4}"/>
-    <hyperlink ref="C47" r:id="rId44" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{E8D257A9-FD31-4556-9D03-E4796389E8CF}"/>
-    <hyperlink ref="C48" r:id="rId45" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{3BAE7E0A-F73A-424A-8068-DC4AC7E0F915}"/>
-    <hyperlink ref="C49" r:id="rId46" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{68445C53-CDB9-499A-A3E8-E8B5A1E21A83}"/>
-    <hyperlink ref="C50" r:id="rId47" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{11E20F1C-82A5-420E-AA26-2D5D508601EC}"/>
-    <hyperlink ref="C51" r:id="rId48" tooltip="Tower of Hanoi" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{BF2BEB75-D5DF-4FA2-914C-04333CB7AA13}"/>
-    <hyperlink ref="C52" r:id="rId49" tooltip="Tower of Hanoi" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{4916F6EB-2ECD-4B5B-BDBE-8DCF6083845C}"/>
-    <hyperlink ref="C53" r:id="rId50" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{FE446E1B-5757-4823-A244-D0B1300D92F9}"/>
-    <hyperlink ref="C56" r:id="rId51" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{69A025E2-E877-403E-AEB1-D03779CE3BD3}"/>
-    <hyperlink ref="C57" r:id="rId52" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{8DD4B752-81CD-476A-A302-914DA46B4526}"/>
-    <hyperlink ref="C58" r:id="rId53" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{8CE8B8B1-FFA3-4F4B-A40C-7CF8B083DE68}"/>
-    <hyperlink ref="C59" r:id="rId54" display="https://codeforces.com/problemset/problem/1426/A" xr:uid="{F5398A26-BC0E-4FC5-8E4F-037D9E83B04B}"/>
-    <hyperlink ref="C60" r:id="rId55" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{48CA6B71-2DF1-48F8-A472-2B53C9D01679}"/>
-    <hyperlink ref="C61" r:id="rId56" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{8B5BB8D9-62F2-4FE9-87D6-D4446B77690F}"/>
-    <hyperlink ref="C62" r:id="rId57" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{2846BE09-AA66-4007-B571-52DE98E45B6E}"/>
-    <hyperlink ref="C63" r:id="rId58" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{08D2B114-CEFA-4DFF-BA59-5AC176658839}"/>
-    <hyperlink ref="C64" r:id="rId59" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{79486861-F18D-487F-8024-C30B4090EB7E}"/>
-    <hyperlink ref="C65" r:id="rId60" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{C227E655-E95E-49EE-8D5A-44194BC60BAF}"/>
-    <hyperlink ref="C66" r:id="rId61" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{25AEB0D9-8985-435C-8381-9419B5BFD25E}"/>
-    <hyperlink ref="C67" r:id="rId62" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{07F5C312-B688-4C66-A197-85CA254A7213}"/>
-    <hyperlink ref="C68" r:id="rId63" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{5D539FAF-75F6-4F01-86CF-344954E6869E}"/>
-    <hyperlink ref="C69" r:id="rId64" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{411C3C51-F0EE-4C44-AFE9-D8DDBBDC526D}"/>
-    <hyperlink ref="C70" r:id="rId65" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{D8A2FA0E-9E00-4904-BD54-F10759F97C5C}"/>
-    <hyperlink ref="C71" r:id="rId66" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{016D1C51-0CA0-42C8-8CCD-22F503298C20}"/>
-    <hyperlink ref="C72" r:id="rId67" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{9AC42B8E-1628-42CE-817A-8EC030DAFAF0}"/>
-    <hyperlink ref="C73" r:id="rId68" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{5F3D28AC-4F74-45DD-8BAD-A50843469889}"/>
-    <hyperlink ref="C74" r:id="rId69" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{005981BE-6BA5-49FC-AD70-CC8707D378DC}"/>
-    <hyperlink ref="C75" r:id="rId70" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{83491A38-5705-45C0-91B1-8A556B777AC7}"/>
-    <hyperlink ref="C76" r:id="rId71" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{910AB615-66E6-4C33-8066-FADE336BCFB3}"/>
-    <hyperlink ref="C77" r:id="rId72" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{1D214953-1B27-4671-BF41-C673CF7441BC}"/>
-    <hyperlink ref="C78" r:id="rId73" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{4F90B0CC-0D3D-4F59-88E9-12B02E52E8E7}"/>
-    <hyperlink ref="C79" r:id="rId74" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{56A00F87-57F5-45AE-82AB-9FA650EB7610}"/>
-    <hyperlink ref="C80" r:id="rId75" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{342465DA-2746-4C09-9380-76A5C4CD2470}"/>
-    <hyperlink ref="C81" r:id="rId76" display="https://codeforces.com/problemset/problem/1107/B" xr:uid="{FF7048A4-C350-4F55-9D3B-498D94EC1FDD}"/>
-    <hyperlink ref="C82" r:id="rId77" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{FFFD0F4C-C55F-4292-B036-4E69A6F4AEC3}"/>
-    <hyperlink ref="C83" r:id="rId78" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{91720979-11D8-450A-BBE0-AD7BC590F5E4}"/>
-    <hyperlink ref="C84" r:id="rId79" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{A7993C35-87EF-4D57-B068-CAEF63F66A3D}"/>
-    <hyperlink ref="C85" r:id="rId80" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{0403F257-6EB2-4A7B-A87D-067D1AB2D551}"/>
-    <hyperlink ref="C86" r:id="rId81" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{6BCF84E3-A284-461A-86DE-53FDC72603A7}"/>
-    <hyperlink ref="C87" r:id="rId82" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{9F7A1ED6-D8B7-426A-9086-83607E4C549D}"/>
-    <hyperlink ref="C88" r:id="rId83" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{C5C1BBCF-9818-47A4-A233-B50FA9429233}"/>
-    <hyperlink ref="C89" r:id="rId84" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{224B315D-650D-49C7-897B-684432B22F89}"/>
-    <hyperlink ref="C90" r:id="rId85" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{82BCBC6B-9EEA-43C3-950D-B2267C954D25}"/>
-    <hyperlink ref="C91" r:id="rId86" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{DB40ECA1-59DD-4A7B-95A1-A9EB2BF1DE3F}"/>
-    <hyperlink ref="C92" r:id="rId87" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{B6DB19D7-35BC-4E8D-80B6-905A038CCDEF}"/>
-    <hyperlink ref="C93" r:id="rId88" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{6A7ECF2E-C033-476C-B046-4FDA56F795E4}"/>
-    <hyperlink ref="C94" r:id="rId89" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{3F662E96-0799-4FB3-85A6-8A40908F6D4B}"/>
-    <hyperlink ref="C95" r:id="rId90" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{838296D1-8F95-4A64-9633-4CCD40CBB151}"/>
-    <hyperlink ref="C96" r:id="rId91" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{7127B025-A0C4-4036-AAAE-1152AC06B63E}"/>
-    <hyperlink ref="C97" r:id="rId92" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{FFA75A85-BBF5-42B3-B599-9417443FBD93}"/>
-    <hyperlink ref="C98" r:id="rId93" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{498B3AC6-DED0-47D4-BEBF-E63ABA70E37D}"/>
-    <hyperlink ref="C99" r:id="rId94" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{AD351C80-0F1F-4D3E-BBD6-EC9D4FE819BB}"/>
-    <hyperlink ref="C100" r:id="rId95" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{18DEE90D-BDE3-49FB-817F-FFDE65FDCA04}"/>
-    <hyperlink ref="C101" r:id="rId96" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{D80F8E0E-72AD-466F-A8F1-5C06C34C7BD1}"/>
-    <hyperlink ref="C102" r:id="rId97" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{02157ABA-151C-4CF3-BE0F-5AA8640AF272}"/>
-    <hyperlink ref="C103" r:id="rId98" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{C6BD44CB-9E98-4D28-9BC1-164A6DC5AA93}"/>
-    <hyperlink ref="C104" r:id="rId99" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{5F4217AB-CB1F-4C58-952A-B2A3F6FE88EA}"/>
-    <hyperlink ref="C105" r:id="rId100" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{F1580A24-ABC6-405F-A44F-1F71FFE9DCDB}"/>
-    <hyperlink ref="C109" r:id="rId101" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{B7C58112-EE76-4593-9BA5-DCF1E3CD8AAE}"/>
-    <hyperlink ref="C110" r:id="rId102" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{00042F64-E8FA-423E-A177-24E7B6CEAB20}"/>
-    <hyperlink ref="C111" r:id="rId103" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{A8BDA395-7C69-4595-93FC-0282E0EFD4E3}"/>
-    <hyperlink ref="C112" r:id="rId104" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{D6D9789B-7968-41B9-B62A-C423BF937181}"/>
-    <hyperlink ref="C115" r:id="rId105" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{061F3928-7A09-48B4-8CBD-F5E169A283D4}"/>
-    <hyperlink ref="C116" r:id="rId106" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{7E02D882-E8DC-445B-8635-209825DCD6EE}"/>
-    <hyperlink ref="C117" r:id="rId107" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{D2E8D740-110B-4878-AD6C-1069825FA10B}"/>
-    <hyperlink ref="C118" r:id="rId108" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{F4261348-260E-4878-AE51-A1F0E1ED6298}"/>
-    <hyperlink ref="C121" r:id="rId109" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{B75C0EEC-FB79-4365-9EF9-4AAE5EC18F0F}"/>
-    <hyperlink ref="C122" r:id="rId110" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{0343B5CD-2F39-496E-92EF-FFE8FAF89D33}"/>
-    <hyperlink ref="C123" r:id="rId111" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{B9439D45-4675-42A0-82E7-91C154AC315C}"/>
-    <hyperlink ref="C124" r:id="rId112" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{AD186EAE-0FD8-4216-BF6F-5DE61E6C4F34}"/>
-    <hyperlink ref="C128" r:id="rId113" display="https://codeforces.com/contest/1370/problem/D" xr:uid="{A9BC2B41-3BCE-4E0C-8903-18F26C75DAD5}"/>
-    <hyperlink ref="C129" r:id="rId114" display="https://www.spoj.com/problems/TDPRIMES/" xr:uid="{9B8F96FB-D014-4380-AE5B-DCE44ABBAE96}"/>
-    <hyperlink ref="C130" r:id="rId115" display="https://www.spoj.com/problems/TDKPRIME/" xr:uid="{A7ABD4EB-BB21-4BC7-B624-06822DF33628}"/>
-    <hyperlink ref="C133" r:id="rId116" display="https://codeforces.com/contest/264/problem/B" xr:uid="{2765188F-D0D3-4B70-AD44-DBE5982EEB5A}"/>
-    <hyperlink ref="C134" r:id="rId117" display="https://codeforces.com/contest/735/problem/D" xr:uid="{D11505DB-7FE5-4015-AEF4-DA8106DD73E4}"/>
-    <hyperlink ref="C135" r:id="rId118" display="https://codeforces.com/contest/546/problem/D" xr:uid="{927CF4E1-9280-4408-93D0-DA69A9DAE8B0}"/>
-    <hyperlink ref="C136" r:id="rId119" display="https://codeforces.com/contest/222/problem/C" xr:uid="{F45A9FC6-52AA-4C68-9F76-8C19E7A13337}"/>
-    <hyperlink ref="C139" r:id="rId120" display="https://codeforces.com/problemset/problem/111/B" xr:uid="{BD609E2F-00A3-4A22-962F-E2D71C4A6D2E}"/>
-    <hyperlink ref="C140" r:id="rId121" display="https://codeforces.com/contest/1228/problem/C" xr:uid="{AA2E00E3-E993-4A6C-B471-4C76238D8063}"/>
-    <hyperlink ref="C141" r:id="rId122" display="https://codeforces.com/contest/1101/problem/D" xr:uid="{487DB7AF-AA15-4D4A-AB33-D91F5A4E1D86}"/>
-    <hyperlink ref="C145" r:id="rId123" display="https://codeforces.com/contest/1101/problem/D" xr:uid="{69594BDD-9D03-427E-9CB8-2E59A9111DD6}"/>
-    <hyperlink ref="C146" r:id="rId124" display="https://codeforces.com/problemset/problem/1594/B" xr:uid="{2872A028-6961-45D2-9F0A-7D669A2A65A2}"/>
-    <hyperlink ref="C147" r:id="rId125" display="https://codeforces.com/problemset/problem/1097/B" xr:uid="{F35596D7-C6C5-4E41-91E3-9F544BA72DE2}"/>
-    <hyperlink ref="C148" r:id="rId126" display="https://codeforces.com/contest/1602/problem/C" xr:uid="{8BFAC610-8856-44FA-9D80-167E4CFCC1CE}"/>
-    <hyperlink ref="C151" r:id="rId127" display="https://codeforces.com/problemset/problem/1095/C" xr:uid="{1052D211-0002-4ABD-BDBB-29D157AE6D1C}"/>
-    <hyperlink ref="C152" r:id="rId128" display="https://codeforces.com/problemset/problem/1494/B" xr:uid="{B5B8DCD0-E3C2-49B6-A69D-42DA41CB969E}"/>
-    <hyperlink ref="C153" r:id="rId129" display="https://codeforces.com/problemset/problem/1151/B" xr:uid="{CACD7565-91A6-4BD5-BC35-F3026B28F957}"/>
-    <hyperlink ref="C154" r:id="rId130" display="https://codeforces.com/problemset/problem/1225/C" xr:uid="{B717C621-3A69-4F5D-A616-853A14EDD8D5}"/>
-    <hyperlink ref="C157" r:id="rId131" display="https://codeforces.com/contest/1174/problem/D" xr:uid="{B41C2DE8-A239-40ED-A335-0C54ABB05668}"/>
-    <hyperlink ref="C158" r:id="rId132" display="https://codeforces.com/problemset/problem/1391/D" xr:uid="{6E115254-7035-4C9C-AA55-597B62FEC7AB}"/>
-    <hyperlink ref="C159" r:id="rId133" display="https://codeforces.com/problemset/problem/1491/D" xr:uid="{3AB9C53F-82AF-4E12-AD3D-076DE1F7BF63}"/>
-    <hyperlink ref="C163" r:id="rId134" display="https://codeforces.com/contest/343/problem/B" xr:uid="{60891248-7B8C-4617-B77F-ACFE7677F2E9}"/>
-    <hyperlink ref="C164" r:id="rId135" display="https://codeforces.com/contest/158/problem/C" xr:uid="{50E32397-6D45-4B01-987A-D19825EC78E2}"/>
-    <hyperlink ref="C165" r:id="rId136" display="https://codeforces.com/contest/5/problem/C" xr:uid="{8ABF07A6-A243-4672-BFEF-4CFED43512B1}"/>
-    <hyperlink ref="C168" r:id="rId137" display="https://codeforces.com/contest/359/problem/D" xr:uid="{D7E9C3C4-E2F0-4A30-825F-81AE50FE6EB1}"/>
-    <hyperlink ref="C169" r:id="rId138" display="https://codeforces.com/contest/1092/problem/D1" xr:uid="{EA699C53-903F-45EA-941F-2A8DB25652A0}"/>
-    <hyperlink ref="C170" r:id="rId139" display="https://codeforces.com/contest/1313/problem/C2" xr:uid="{91C3E5D5-7199-4582-8613-1C5660DDE26A}"/>
-    <hyperlink ref="C171" r:id="rId140" display="https://codeforces.com/contest/1515/problem/C" xr:uid="{9600B657-7CED-4AEF-9997-3E58B777B4FC}"/>
-    <hyperlink ref="C174" r:id="rId141" display="https://codeforces.com/contest/319/problem/B" xr:uid="{63920447-6665-42B4-9750-0A8A96E20038}"/>
-    <hyperlink ref="C175" r:id="rId142" display="https://codeforces.com/contest/487/problem/B" xr:uid="{2B512440-7FD9-41E9-9F0A-F5847F1CB9CC}"/>
-    <hyperlink ref="C176" r:id="rId143" display="https://codeforces.com/contest/1092/problem/D2" xr:uid="{47843149-CAA3-453B-84F6-C5990E504EB9}"/>
-    <hyperlink ref="C177" r:id="rId144" display="https://codeforces.com/contest/1156/problem/E" xr:uid="{10AD5C70-4E84-4C2C-A8DA-32A9D35DBADB}"/>
-    <hyperlink ref="C178" r:id="rId145" display="https://codeforces.com/contest/911/problem/E" xr:uid="{8604D6DD-DE06-4185-9618-1AB590B54309}"/>
-    <hyperlink ref="C179" r:id="rId146" display="https://codeforces.com/contest/507/problem/E?locale=en" xr:uid="{C050C26C-B665-41F3-957A-454CCEB3FFE8}"/>
-    <hyperlink ref="C183" r:id="rId147" display="https://codeforces.com/problemset/problem/271/D" xr:uid="{44A3B5D5-C6D4-4399-9FC0-56461D4260AC}"/>
-    <hyperlink ref="C184" r:id="rId148" display="https://codeforces.com/contest/1326/problem/D2" xr:uid="{715E2A38-958E-4788-9451-A3ABCFB20DE6}"/>
-    <hyperlink ref="C185" r:id="rId149" display="https://codeforces.com/contest/514/problem/C" xr:uid="{94FDA7D8-67B3-4DD3-810D-19A86C4B1C17}"/>
-    <hyperlink ref="C186" r:id="rId150" display="https://codeforces.com/contest/7/problem/D" xr:uid="{6ACAA64C-0929-4476-99D0-CD08CC2E2414}"/>
-    <hyperlink ref="C187" r:id="rId151" display="https://codeforces.com/contest/514/problem/C" xr:uid="{6701AE01-6DFC-4B04-9FE8-A33268FE31C1}"/>
-    <hyperlink ref="C188" r:id="rId152" display="https://codeforces.com/contest/633/problem/C" xr:uid="{00B2BD2E-717A-4E06-819B-C22FAC98720A}"/>
-    <hyperlink ref="C191" r:id="rId153" display="https://codeforces.com/contest/1016/problem/B" xr:uid="{4C80B6E8-2C12-425A-8ED9-1707185AF4B7}"/>
-    <hyperlink ref="C192" r:id="rId154" display="https://codeforces.com/contest/471/problem/D" xr:uid="{9C5B0546-C5C6-4FA5-8AE7-2D9B6E0D4D96}"/>
-    <hyperlink ref="C193" r:id="rId155" display="https://codeforces.com/problemset/problem/126/B" xr:uid="{F87A64E5-3538-419C-9A0C-57FB1FFE7C4B}"/>
-    <hyperlink ref="C194" r:id="rId156" display="https://codeforces.com/contest/471/problem/D" xr:uid="{A0AC9302-3D99-44D2-9354-D83D66F3CE2A}"/>
-    <hyperlink ref="C195" r:id="rId157" display="https://codeforces.com/contest/1138/problem/D" xr:uid="{3475B623-6F0C-46A1-8FCD-93EF1DD7BEB8}"/>
-    <hyperlink ref="C196" r:id="rId158" display="https://codeforces.com/contest/126/problem/B" xr:uid="{71E8E9B9-F0E6-4A7D-B28B-238F5C6E3377}"/>
-    <hyperlink ref="C197" r:id="rId159" display="https://codeforces.com/contest/432/problem/D" xr:uid="{EF947049-8495-4B21-995C-8EC9A2D81E51}"/>
-    <hyperlink ref="C198" r:id="rId160" display="https://codeforces.com/contest/1537/problem/E2" xr:uid="{18239E1F-8DBB-4DCB-8748-9E74DE91E313}"/>
-    <hyperlink ref="C201" r:id="rId161" display="https://www.spoj.com/problems/NUMOFPAL/" xr:uid="{323E93AB-1832-45B5-BF32-41914A1391DA}"/>
-    <hyperlink ref="C202" r:id="rId162" display="https://www.spoj.com/problems/LPS/" xr:uid="{9B4DB6E4-6F3B-4EEA-8222-DAE9C031EE19}"/>
-    <hyperlink ref="C203" r:id="rId163" display="https://www.spoj.com/problems/MSUBSTR/" xr:uid="{0DA58C82-02FD-40CC-808D-2F89C48EDA0D}"/>
-    <hyperlink ref="C204" r:id="rId164" display="https://www.spoj.com/problems/EPALIN/" xr:uid="{9051C92C-A2C5-4EAB-8774-DCCAFA384F99}"/>
-    <hyperlink ref="C205" r:id="rId165" display="https://codeforces.com/contest/1080/problem/E" xr:uid="{1A22C955-CBCB-402C-BA4C-05DFDBBC3E0D}"/>
-    <hyperlink ref="C208" r:id="rId166" display="https://codeforces.com/problemset/problem/1006/F" xr:uid="{5DB7211F-15E1-4360-95DA-35051BDFB59A}"/>
-    <hyperlink ref="C212" r:id="rId167" display="https://cses.fi/problemset/task/1674" xr:uid="{7FFB5365-1980-470D-894F-4201C72C5B8B}"/>
-    <hyperlink ref="C213" r:id="rId168" display="https://cses.fi/problemset/task/1130" xr:uid="{FF3A5286-BDE1-4F90-A26B-CC3D774CDED5}"/>
-    <hyperlink ref="C214" r:id="rId169" display="https://codeforces.com/gym/102694/problem/A" xr:uid="{9380042F-2697-4EBF-A306-633B58E2659E}"/>
-    <hyperlink ref="C215" r:id="rId170" display="https://codeforces.com/gym/102694/problem/B" xr:uid="{DD89A320-B792-4BC4-BEA4-C93936F7BD2E}"/>
-    <hyperlink ref="C218" r:id="rId171" display="https://codeforces.com/gym/102694/problem/A" xr:uid="{ED37F328-7516-4CF5-9CD5-16B6914F95C6}"/>
-    <hyperlink ref="C219" r:id="rId172" display="https://cses.fi/problemset/task/1133" xr:uid="{DDB64992-5418-42DE-8679-F1618F85EAD8}"/>
-    <hyperlink ref="C220" r:id="rId173" display="https://codeforces.com/contest/1294/problem/F" xr:uid="{A149CC9E-6043-4EA3-A74D-823754D9461A}"/>
-    <hyperlink ref="C225" r:id="rId174" display="https://codeforces.com/gym/102694/problem/C" xr:uid="{E7F43E13-BFC6-4B09-86D9-FB2267C1BECA}"/>
-    <hyperlink ref="C226" r:id="rId175" display="https://codeforces.com/gym/102694/problem/D" xr:uid="{F714D048-6AAF-4EA0-BA78-D650D77FBCFF}"/>
-    <hyperlink ref="C230" r:id="rId176" display="https://codeforces.com/contest/1328/problem/E" xr:uid="{76E17511-72BA-49E3-9250-D5784BEC974B}"/>
-    <hyperlink ref="C231" r:id="rId177" display="https://codeforces.com/contest/1304/problem/E" xr:uid="{FF4FA1F2-B40E-4FA3-A656-2B30BE7572D8}"/>
-    <hyperlink ref="C232" r:id="rId178" display="https://codeforces.com/contest/208/problem/E" xr:uid="{4A4A7A4C-6683-4A5A-9961-6EDD4B58DC98}"/>
-    <hyperlink ref="C233" r:id="rId179" display="https://codeforces.com/contest/191/problem/C" xr:uid="{3FBD5886-F9ED-46A9-B006-D1DC6D17C33F}"/>
-    <hyperlink ref="C237" r:id="rId180" display="https://codeforces.com/contest/519/problem/E" xr:uid="{CED2A27E-BE1F-403F-8128-A51802531F2E}"/>
-    <hyperlink ref="C238" r:id="rId181" display="https://codeforces.com/contest/587/problem/C" xr:uid="{68F8782D-0553-417F-9F79-6296E70263B7}"/>
-    <hyperlink ref="C239" r:id="rId182" display="https://codeforces.com/contest/609/problem/E" xr:uid="{A69F627D-8B97-415C-A36E-22FFEE8C2F38}"/>
-    <hyperlink ref="C240" r:id="rId183" display="https://codeforces.com/contest/466/problem/E" xr:uid="{A9DC7A38-4FFF-43E6-97A7-836F74BE5F87}"/>
-    <hyperlink ref="C244" r:id="rId184" display="https://codeforces.com/gym/102694/problem/E" xr:uid="{2356EAA5-E8F4-4F65-BDF1-53CD27FE09D2}"/>
-    <hyperlink ref="C245" r:id="rId185" display="https://codeforces.com/gym/102694/problem/F" xr:uid="{23220DCA-2714-4BF3-96A5-C116E94A2732}"/>
-    <hyperlink ref="C249" r:id="rId186" display="https://codeforces.com/problemset/problem/520/B" xr:uid="{03CE039F-08B2-4E70-96F8-4BBE007E8F85}"/>
-    <hyperlink ref="C250" r:id="rId187" display="https://codeforces.com/problemset/problem/115/A" xr:uid="{07763546-702A-488F-B361-FF5B07E1B66B}"/>
-    <hyperlink ref="C251" r:id="rId188" display="https://codeforces.com/problemset/problem/580/C" xr:uid="{BDD811C1-5E29-47D3-AAFF-7DDA240C534D}"/>
-    <hyperlink ref="C252" r:id="rId189" display="https://codeforces.com/problemset/problem/977/E" xr:uid="{8DBACEA7-048B-43A2-94BC-E04BEA8F9451}"/>
-    <hyperlink ref="C253" r:id="rId190" display="https://codeforces.com/contest/1144/problem/F" xr:uid="{9FE16E68-8FF3-460E-92B7-DAB7B208FF7C}"/>
-    <hyperlink ref="C254" r:id="rId191" display="https://codeforces.com/contest/510/problem/C" xr:uid="{33A4D3B2-E777-44B9-B84E-459A2ECECACA}"/>
-    <hyperlink ref="C255" r:id="rId192" display="https://codeforces.com/contest/20/problem/C" xr:uid="{D127B550-ED72-4E18-A082-F576D3C4BA4E}"/>
-    <hyperlink ref="C256" r:id="rId193" display="https://codeforces.com/problemset/problem/475/B" xr:uid="{70DCAABE-9F1B-4729-86FF-8B1CB3AF8E26}"/>
-    <hyperlink ref="C259" r:id="rId194" display="https://codeforces.com/contest/986/problem/A" xr:uid="{D02ECCA4-F730-448F-B6F1-939563C28D14}"/>
-    <hyperlink ref="C260" r:id="rId195" display="https://codeforces.com/contest/242/problem/C" xr:uid="{FD61155A-7608-4817-A8B3-3F717CFB1439}"/>
-    <hyperlink ref="C261" r:id="rId196" display="https://codeforces.com/contest/1345/problem/D" xr:uid="{384CC8F1-B40A-489B-AC88-53B0429E03BA}"/>
-    <hyperlink ref="C262" r:id="rId197" display="https://codeforces.com/contest/229/problem/B" xr:uid="{1FD52FED-045C-409F-8E53-06D049A34D17}"/>
-    <hyperlink ref="C263" r:id="rId198" display="https://codeforces.com/contest/1385/problem/E" xr:uid="{EE15E94D-9D36-4C47-B417-1675FA127C6B}"/>
-    <hyperlink ref="C264" r:id="rId199" display="https://codeforces.com/contest/295/problem/B" xr:uid="{0DC2B729-DC20-4842-A7A7-719CFDB205D7}"/>
-    <hyperlink ref="C265" r:id="rId200" display="https://codeforces.com/contest/1213/problem/F" xr:uid="{13C08E4F-BC6F-4401-84F4-30EE7AAE25AE}"/>
-    <hyperlink ref="C266" r:id="rId201" display="https://codeforces.com/contest/1343/problem/E" xr:uid="{F05DEB4E-A305-474F-9DCB-E47B747BC2AF}"/>
-    <hyperlink ref="C267" r:id="rId202" display="https://codeforces.com/contest/1296/problem/E1" xr:uid="{6380A587-6E91-4CA2-9898-0CF85961D8DF}"/>
-    <hyperlink ref="C270" r:id="rId203" display="https://codeforces.com/contest/1573/problem/C" xr:uid="{172ADCDE-5E1B-46A8-A8CD-A1F3A6C4598A}"/>
-    <hyperlink ref="C271" r:id="rId204" display="https://codeforces.com/contest/1547/problem/G" xr:uid="{68D336F3-BAAD-4EBC-83E5-000235EEE4AF}"/>
-    <hyperlink ref="C272" r:id="rId205" display="https://codeforces.com/contest/229/problem/B" xr:uid="{35855A60-5E9C-4A54-A606-899BDB16A77F}"/>
-    <hyperlink ref="C273" r:id="rId206" display="https://codeforces.com/contest/400/problem/D" xr:uid="{72DC67D7-EAEE-4D38-B99F-38FE9CE0C123}"/>
-    <hyperlink ref="C274" r:id="rId207" display="https://codeforces.com/contest/178/problem/B3" xr:uid="{7FF1E0ED-2F07-4EB3-AD0E-59EDAC055801}"/>
-    <hyperlink ref="C277" r:id="rId208" display="https://codeforces.com/problemset/problem/185/A" xr:uid="{903674CA-0720-4A19-B92F-8AD6DAED854A}"/>
-    <hyperlink ref="C278" r:id="rId209" display="https://codeforces.com/contest/1117/problem/D" xr:uid="{07824635-BA83-4FE1-8CC3-9A6D12288666}"/>
-    <hyperlink ref="C279" r:id="rId210" display="https://codeforces.com/contest/582/problem/B" xr:uid="{10109640-8108-443F-8620-B847F104CB13}"/>
-    <hyperlink ref="C280" r:id="rId211" display="https://codeforces.com/contest/222/problem/E" xr:uid="{D5085D74-6CFD-48DF-AE27-632B639EF9D9}"/>
-    <hyperlink ref="C281" r:id="rId212" display="https://codeforces.com/contest/621/problem/E" xr:uid="{ED16D8F6-66AA-4378-90B1-8A51D3F534FF}"/>
-    <hyperlink ref="C282" r:id="rId213" display="https://codeforces.com/contest/1182/problem/E" xr:uid="{5CB6B1DD-4D4C-4985-9FE7-037910CD3270}"/>
-    <hyperlink ref="C285" r:id="rId214" display="https://codeforces.com/contest/706/problem/D" xr:uid="{48686123-F8FC-43B1-BE84-27098373DAC9}"/>
-    <hyperlink ref="C286" r:id="rId215" display="https://codeforces.com/contest/948/problem/D" xr:uid="{E8923895-166D-4A1F-BB8D-46590BA4DBD6}"/>
-    <hyperlink ref="C287" r:id="rId216" display="https://codeforces.com/contest/665/problem/E" xr:uid="{D7885557-77BE-4E04-990F-C82385E08D44}"/>
-    <hyperlink ref="C288" r:id="rId217" display="https://codeforces.com/contest/1285/problem/D" xr:uid="{32B74896-AD74-486E-A0FF-95C9A142ECB1}"/>
-    <hyperlink ref="C289" r:id="rId218" display="https://codeforces.com/contest/858/problem/D" xr:uid="{8D47675A-9A4E-4455-9BCA-50A06F323245}"/>
-    <hyperlink ref="C290" r:id="rId219" display="https://codeforces.com/contest/455/problem/B" xr:uid="{E0C4AEA9-6B4E-494F-B268-29067F3A3EC8}"/>
-    <hyperlink ref="C291" r:id="rId220" display="https://codeforces.com/contest/113/problem/B" xr:uid="{ED89D802-CE14-4461-A520-8BB9BD8BE1AA}"/>
-    <hyperlink ref="C292" r:id="rId221" display="https://codeforces.com/contest/282/problem/E" xr:uid="{EA845F39-5B96-4069-8B21-983DBC58DF14}"/>
-    <hyperlink ref="C296" r:id="rId222" display="https://codeforces.com/problemset/problem/702/A" xr:uid="{E9CB2DE9-88D2-48C8-8177-E4B35AE538A3}"/>
-    <hyperlink ref="C297" r:id="rId223" display="https://codeforces.com/problemset/problem/894/A" xr:uid="{45DD1ECF-6BF4-4EB1-8EB4-A127D524D50A}"/>
-    <hyperlink ref="C298" r:id="rId224" display="https://codeforces.com/problemset/problem/1501/B" xr:uid="{4FBEEB1D-F34E-4C6E-9591-1FA9D23C1A7E}"/>
-    <hyperlink ref="C299" r:id="rId225" display="https://codeforces.com/problemset/problem/1469/B" xr:uid="{435C14CC-3600-4444-BB39-C07F61F30FB8}"/>
-    <hyperlink ref="C300" r:id="rId226" display="https://codeforces.com/problemset/problem/363/B" xr:uid="{BA1030A2-0B68-42AE-AB50-216C4203E3E9}"/>
-    <hyperlink ref="C301" r:id="rId227" display="https://codeforces.com/problemset/problem/313/B" xr:uid="{BC5B1306-257D-44A1-8624-5505A9EB40C7}"/>
-    <hyperlink ref="C302" r:id="rId228" display="https://codeforces.com/problemset/problem/327/A" xr:uid="{5BD0C670-1BFF-49BF-A382-3E757D216AAD}"/>
-    <hyperlink ref="C303" r:id="rId229" display="https://codeforces.com/problemset/problem/961/B" xr:uid="{8A379A09-06DF-4F8D-8DD8-5C5124AB00D7}"/>
-    <hyperlink ref="C304" r:id="rId230" display="https://codeforces.com/problemset/problem/522/A" xr:uid="{FF5DD54E-F619-46DF-B65B-A27FAD9EFA1F}"/>
-    <hyperlink ref="C305" r:id="rId231" display="https://codeforces.com/problemset/problem/1042/B" xr:uid="{1185A058-2C9D-4BA9-A28F-FB887BFEE948}"/>
-    <hyperlink ref="C306" r:id="rId232" display="https://codeforces.com/problemset/problem/189/A" xr:uid="{4D886BB8-3373-44B4-B08A-E3F5CAA5264C}"/>
-    <hyperlink ref="C307" r:id="rId233" display="https://codeforces.com/problemset/problem/1420/C1" xr:uid="{CC56CF98-4333-4B42-8952-08D42456AEF4}"/>
-    <hyperlink ref="C308" r:id="rId234" display="https://codeforces.com/problemset/problem/414/B" xr:uid="{BA3CB3F1-8EF6-47D4-A88E-63C6AEA83989}"/>
-    <hyperlink ref="C309" r:id="rId235" display="https://codeforces.com/problemset/problem/1195/C" xr:uid="{12D783EC-8F92-4786-ABCF-CCC4C791CC68}"/>
-    <hyperlink ref="C310" r:id="rId236" display="https://codeforces.com/problemset/problem/1350/B" xr:uid="{3F0BEA35-B386-4831-9BAF-0EAEA90475CA}"/>
-    <hyperlink ref="C313" r:id="rId237" display="https://codeforces.com/contest/505/problem/C" xr:uid="{A34BB500-070D-46A4-82C9-18161C0DD247}"/>
-    <hyperlink ref="C314" r:id="rId238" display="https://codeforces.com/contest/577/problem/B" xr:uid="{C84FF700-349E-48AC-B275-E3F3056D2F3C}"/>
-    <hyperlink ref="C315" r:id="rId239" display="https://codeforces.com/contest/204/problem/A" xr:uid="{91186E77-D348-48B6-8451-4FFC525AEC89}"/>
-    <hyperlink ref="C316" r:id="rId240" display="https://codeforces.com/contest/448/problem/C" xr:uid="{F22C51E8-1F52-47C6-BBD7-ECD4C3D616B6}"/>
-    <hyperlink ref="C317" r:id="rId241" display="https://codeforces.com/contest/479/problem/E" xr:uid="{28718124-3B57-4951-9AAA-E47240184D16}"/>
-    <hyperlink ref="C318" r:id="rId242" display="https://codeforces.com/contest/401/problem/D" xr:uid="{8A721A57-1986-457A-8021-87A60BC9E699}"/>
-    <hyperlink ref="C319" r:id="rId243" display="https://codeforces.com/contest/777/problem/E" xr:uid="{F86235DE-3239-4B04-A0FD-C5AC87EAE1D4}"/>
-    <hyperlink ref="C320" r:id="rId244" display="https://codeforces.com/contest/1036/problem/C" xr:uid="{ABFBFFD1-073A-401C-8C5D-97E718137EBF}"/>
-    <hyperlink ref="C321" r:id="rId245" display="https://codeforces.com/contest/219/problem/D" xr:uid="{FE90156B-2AA2-40BA-AFEB-83DADB93039D}"/>
-    <hyperlink ref="C322" r:id="rId246" display="https://codeforces.com/contest/337/problem/D" xr:uid="{28820F82-1B1E-47ED-87E2-A974AFF3E684}"/>
-    <hyperlink ref="C325" r:id="rId247" display="https://codeforces.com/contest/165/problem/E" xr:uid="{F68F6AFD-FA8C-4D3A-A69B-42B31D25653D}"/>
-    <hyperlink ref="C326" r:id="rId248" display="https://codeforces.com/contest/687/problem/C" xr:uid="{3FA5A113-AFCF-441C-BD48-A1CF8C9DDB26}"/>
-    <hyperlink ref="C327" r:id="rId249" display="https://codeforces.com/contest/1132/problem/F" xr:uid="{F4643E28-4C15-45FC-A72A-508D9CE7C22F}"/>
-    <hyperlink ref="C328" r:id="rId250" display="https://codeforces.com/contest/1253/problem/E" xr:uid="{0CA1D004-898E-4052-BCB3-54F2911052DA}"/>
-    <hyperlink ref="C329" r:id="rId251" display="https://codeforces.com/contest/1216/problem/F" xr:uid="{7E93F84E-E741-4BBC-9E99-025DE5BFBD25}"/>
-    <hyperlink ref="C330" r:id="rId252" display="https://codeforces.com/contest/461/problem/B" xr:uid="{2DAB43C0-BC57-4F91-9E77-E0838FA70381}"/>
-    <hyperlink ref="C331" r:id="rId253" display="https://codeforces.com/contest/319/problem/C" xr:uid="{AEB06620-C1E7-4211-B3D4-B60C1779E691}"/>
-    <hyperlink ref="C332" r:id="rId254" display="https://codeforces.com/contest/1083/problem/E" xr:uid="{7F0B980C-F0C8-43DD-8BA6-C856B3205FD7}"/>
-    <hyperlink ref="C333" r:id="rId255" display="https://codeforces.com/contest/507/problem/D" xr:uid="{B41A95E1-F69F-4364-8ACE-0144A1D1C644}"/>
-    <hyperlink ref="C334" r:id="rId256" display="https://codeforces.com/contest/540/problem/D" xr:uid="{208ADE34-2713-4257-80F8-DBB8D5F837B8}"/>
-    <hyperlink ref="C338" r:id="rId257" display="https://codeforces.com/problemset/problem/1534/C" xr:uid="{C702161A-8805-47E1-8225-74639226D8E2}"/>
-    <hyperlink ref="C339" r:id="rId258" display="https://codeforces.com/problemset/problem/217/A" xr:uid="{EC12BDBD-4FFD-49A1-83E6-BFBCBCB07A4B}"/>
-    <hyperlink ref="C340" r:id="rId259" display="https://codeforces.com/contest/277/problem/A" xr:uid="{DCBF8D08-1CCB-49AB-BB96-C5694048DEE5}"/>
-    <hyperlink ref="C343" r:id="rId260" display="https://codeforces.com/contest/884/problem/C" xr:uid="{689CFB1A-E1C1-4E26-B3E3-418CAA5A6D0E}"/>
-    <hyperlink ref="C344" r:id="rId261" display="https://codeforces.com/contest/1332/problem/C" xr:uid="{EE66C364-1C95-4220-B361-C8FF433F9404}"/>
-    <hyperlink ref="C345" r:id="rId262" display="https://codeforces.com/contest/455/problem/C" xr:uid="{634B5492-0C59-41F6-990B-84E1DC600A37}"/>
-    <hyperlink ref="C348" r:id="rId263" display="https://codeforces.com/contest/1156/problem/D" xr:uid="{6EF110B4-33FA-4F45-8FF2-9F13DABF1BB4}"/>
-    <hyperlink ref="C349" r:id="rId264" display="https://codeforces.com/contest/1213/problem/G" xr:uid="{A56E2B52-F95B-4ECA-8659-EDA02DF7ABD3}"/>
-    <hyperlink ref="C350" r:id="rId265" display="https://codeforces.com/problemset/problem/1494/D" xr:uid="{6F2E5012-EEAE-49ED-A2F3-FE16C3ECB4D6}"/>
-    <hyperlink ref="C351" r:id="rId266" display="https://codeforces.com/problemset/problem/455/C" xr:uid="{A267F2D5-B666-44E0-B422-78D2B4831B43}"/>
-    <hyperlink ref="C354" r:id="rId267" display="https://codeforces.com/problemset/problem/455/C" xr:uid="{BDB565D4-77CE-4F3F-8B12-B5D154D3A474}"/>
-    <hyperlink ref="C355" r:id="rId268" display="https://codeforces.com/contest/617/problem/E" xr:uid="{D9653234-537C-439C-A89E-6AAF59570145}"/>
-    <hyperlink ref="C356" r:id="rId269" display="https://codeforces.com/contest/220/problem/B" xr:uid="{BE689AA3-70EE-4631-9831-178D5A6365A1}"/>
-    <hyperlink ref="C357" r:id="rId270" display="https://codeforces.com/contest/1514/problem/D" xr:uid="{8D3CA309-A854-42B3-9C84-D1AC96176234}"/>
-    <hyperlink ref="C358" r:id="rId271" display="https://codeforces.com/contest/375/problem/D" xr:uid="{FF786C16-8978-4A96-863F-C1D3A1D33F0E}"/>
-    <hyperlink ref="C359" r:id="rId272" display="https://codeforces.com/contest/242/problem/E" xr:uid="{4F1239AB-D143-4DBA-8F2B-B80B8888794A}"/>
-    <hyperlink ref="C362" r:id="rId273" display="https://codeforces.com/contest/61/problem/E" xr:uid="{8EF670D2-1707-410B-AAA1-312462EEA484}"/>
-    <hyperlink ref="C363" r:id="rId274" display="https://codeforces.com/contest/1311/problem/F" xr:uid="{FF0F8182-D5D0-4195-93D3-3AF36451C3A2}"/>
-    <hyperlink ref="C364" r:id="rId275" display="https://codeforces.com/contest/283/problem/A" xr:uid="{8243D1D2-CA64-4DAC-B265-4AA1A2412FE2}"/>
-    <hyperlink ref="C365" r:id="rId276" display="https://codeforces.com/contest/459/problem/D" xr:uid="{47EA03F6-03CF-4D3B-91AB-75C6C77DF2A0}"/>
-    <hyperlink ref="C366" r:id="rId277" display="https://codeforces.com/contest/340/problem/D" xr:uid="{187067DD-D539-4AFB-A27C-FF3B00381C73}"/>
-    <hyperlink ref="C367" r:id="rId278" display="https://codeforces.com/contest/1076/problem/E" xr:uid="{D5C6E09A-F164-4AF7-9870-53165C652E17}"/>
-    <hyperlink ref="C368" r:id="rId279" display="https://codeforces.com/contest/1354/problem/D" xr:uid="{2FCBF469-5C35-4CDD-8CF1-D7214D125C9A}"/>
-    <hyperlink ref="C369" r:id="rId280" display="https://codeforces.com/contest/1405/problem/E" xr:uid="{E76E6E9E-7419-4F9F-8210-26E2ED06CFF2}"/>
-    <hyperlink ref="C370" r:id="rId281" display="https://codeforces.com/contest/383/problem/C" xr:uid="{23843970-D3D1-4ED0-B16A-D93BC0596B1E}"/>
-    <hyperlink ref="C371" r:id="rId282" display="https://codeforces.com/contest/1526/problem/D" xr:uid="{D6B904D3-2D5E-46BF-99AF-F1A9BD57E273}"/>
-    <hyperlink ref="C372" r:id="rId283" display="https://codeforces.com/contest/276/problem/E" xr:uid="{3C8EF79E-8952-41B4-98D3-0EED34544C26}"/>
-    <hyperlink ref="C373" r:id="rId284" display="https://codeforces.com/contest/375/problem/D" xr:uid="{018C5B9B-9D8F-4A87-A015-C6AF61D58DB4}"/>
-    <hyperlink ref="C376" r:id="rId285" display="https://codeforces.com/contest/339/problem/D" xr:uid="{007FBF91-F09C-4404-BA7A-E454466AA24D}"/>
-    <hyperlink ref="C377" r:id="rId286" display="https://codeforces.com/contest/914/problem/D" xr:uid="{4A87C3E9-AA02-4EB4-BFE1-D49DB7F24C90}"/>
-    <hyperlink ref="C378" r:id="rId287" display="https://codeforces.com/contest/459/problem/D" xr:uid="{DDCB0CEE-BE07-449A-A01A-AD6D27FB0D33}"/>
-    <hyperlink ref="C379" r:id="rId288" display="https://codeforces.com/contest/61/problem/E" xr:uid="{22095C40-BB89-4376-A758-66AADF897596}"/>
-    <hyperlink ref="C380" r:id="rId289" display="https://codeforces.com/contest/380/problem/C" xr:uid="{E33C2986-BD5E-469C-866B-C7A1155D9185}"/>
-    <hyperlink ref="C381" r:id="rId290" display="https://codeforces.com/contest/474/problem/F" xr:uid="{ADB50F96-7C3A-416C-941B-F281011EB73F}"/>
-    <hyperlink ref="C382" r:id="rId291" display="https://codeforces.com/contest/1237/problem/D" xr:uid="{CA5FB483-8226-41F3-A807-92897DD0AF68}"/>
-    <hyperlink ref="C383" r:id="rId292" display="https://codeforces.com/contest/292/problem/E" xr:uid="{8014A4D0-2FBB-43E7-8E8B-C439C3F885DB}"/>
-    <hyperlink ref="C384" r:id="rId293" display="https://codeforces.com/contest/482/problem/B" xr:uid="{D7001310-52CF-4448-877A-2D82FA553FDB}"/>
-    <hyperlink ref="C385" r:id="rId294" display="https://codeforces.com/contest/1187/problem/D" xr:uid="{A82BD182-2528-4C02-86AE-8506D48094C9}"/>
-    <hyperlink ref="C386" r:id="rId295" display="https://codeforces.com/contest/920/problem/F" xr:uid="{E0E6F155-2F47-4079-A6BE-724897B295EF}"/>
-    <hyperlink ref="C387" r:id="rId296" display="https://codeforces.com/contest/1535/problem/D?locale=en" xr:uid="{BFF507B3-ABFC-412A-8855-FD1D9DAB4404}"/>
-    <hyperlink ref="C388" r:id="rId297" display="https://codeforces.com/contest/438/problem/D?locale=en" xr:uid="{D7D8F26B-28F7-4421-B505-1A50D99C7966}"/>
-    <hyperlink ref="C389" r:id="rId298" display="https://codeforces.com/contest/1556/problem/E" xr:uid="{63AE4160-9A44-45DE-83ED-1C1854964B2B}"/>
-    <hyperlink ref="C390" r:id="rId299" display="https://codeforces.com/contest/1567/problem/E" xr:uid="{066550AD-B9BE-4EC9-B0D3-3C7C7F90F7A1}"/>
-    <hyperlink ref="C393" r:id="rId300" display="https://codeforces.com/contest/52/problem/C" xr:uid="{F7A36424-5B0B-4295-B7AE-41BCAF57DE00}"/>
-    <hyperlink ref="C394" r:id="rId301" display="https://codeforces.com/contest/1023/problem/D" xr:uid="{28BD986E-8622-41B9-A104-58A55C28DDB9}"/>
-    <hyperlink ref="C395" r:id="rId302" display="https://codeforces.com/contest/242/problem/E" xr:uid="{1CA2E82E-F835-4825-A47A-E7A6E0A885CB}"/>
-    <hyperlink ref="C396" r:id="rId303" display="https://codeforces.com/contest/1557/problem/D" xr:uid="{9955F7AD-C0EF-48B4-A08E-FB979B0B1D8C}"/>
-    <hyperlink ref="C397" r:id="rId304" display="https://codeforces.com/contest/145/problem/E" xr:uid="{C5723FFD-146D-497B-97B4-9222F7F8140F}"/>
-    <hyperlink ref="C398" r:id="rId305" display="https://codeforces.com/contest/777/problem/E" xr:uid="{5EF62371-CBD1-4478-ADB5-7390ACE0BE95}"/>
+    <hyperlink ref="C56" r:id="rId1" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{69A025E2-E877-403E-AEB1-D03779CE3BD3}"/>
+    <hyperlink ref="C57" r:id="rId2" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{8DD4B752-81CD-476A-A302-914DA46B4526}"/>
+    <hyperlink ref="C58" r:id="rId3" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{8CE8B8B1-FFA3-4F4B-A40C-7CF8B083DE68}"/>
+    <hyperlink ref="C59" r:id="rId4" display="https://codeforces.com/problemset/problem/1426/A" xr:uid="{F5398A26-BC0E-4FC5-8E4F-037D9E83B04B}"/>
+    <hyperlink ref="C60" r:id="rId5" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{48CA6B71-2DF1-48F8-A472-2B53C9D01679}"/>
+    <hyperlink ref="C61" r:id="rId6" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{8B5BB8D9-62F2-4FE9-87D6-D4446B77690F}"/>
+    <hyperlink ref="C62" r:id="rId7" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{2846BE09-AA66-4007-B571-52DE98E45B6E}"/>
+    <hyperlink ref="C63" r:id="rId8" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{08D2B114-CEFA-4DFF-BA59-5AC176658839}"/>
+    <hyperlink ref="C64" r:id="rId9" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{79486861-F18D-487F-8024-C30B4090EB7E}"/>
+    <hyperlink ref="C65" r:id="rId10" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{C227E655-E95E-49EE-8D5A-44194BC60BAF}"/>
+    <hyperlink ref="C66" r:id="rId11" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{25AEB0D9-8985-435C-8381-9419B5BFD25E}"/>
+    <hyperlink ref="C67" r:id="rId12" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{07F5C312-B688-4C66-A197-85CA254A7213}"/>
+    <hyperlink ref="C68" r:id="rId13" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{5D539FAF-75F6-4F01-86CF-344954E6869E}"/>
+    <hyperlink ref="C69" r:id="rId14" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{411C3C51-F0EE-4C44-AFE9-D8DDBBDC526D}"/>
+    <hyperlink ref="C70" r:id="rId15" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{D8A2FA0E-9E00-4904-BD54-F10759F97C5C}"/>
+    <hyperlink ref="C71" r:id="rId16" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{016D1C51-0CA0-42C8-8CCD-22F503298C20}"/>
+    <hyperlink ref="C72" r:id="rId17" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{9AC42B8E-1628-42CE-817A-8EC030DAFAF0}"/>
+    <hyperlink ref="C73" r:id="rId18" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{5F3D28AC-4F74-45DD-8BAD-A50843469889}"/>
+    <hyperlink ref="C74" r:id="rId19" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{005981BE-6BA5-49FC-AD70-CC8707D378DC}"/>
+    <hyperlink ref="C75" r:id="rId20" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{83491A38-5705-45C0-91B1-8A556B777AC7}"/>
+    <hyperlink ref="C76" r:id="rId21" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{910AB615-66E6-4C33-8066-FADE336BCFB3}"/>
+    <hyperlink ref="C77" r:id="rId22" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{1D214953-1B27-4671-BF41-C673CF7441BC}"/>
+    <hyperlink ref="C78" r:id="rId23" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{4F90B0CC-0D3D-4F59-88E9-12B02E52E8E7}"/>
+    <hyperlink ref="C79" r:id="rId24" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{56A00F87-57F5-45AE-82AB-9FA650EB7610}"/>
+    <hyperlink ref="C80" r:id="rId25" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{342465DA-2746-4C09-9380-76A5C4CD2470}"/>
+    <hyperlink ref="C81" r:id="rId26" display="https://codeforces.com/problemset/problem/1107/B" xr:uid="{FF7048A4-C350-4F55-9D3B-498D94EC1FDD}"/>
+    <hyperlink ref="C82" r:id="rId27" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{FFFD0F4C-C55F-4292-B036-4E69A6F4AEC3}"/>
+    <hyperlink ref="C83" r:id="rId28" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{91720979-11D8-450A-BBE0-AD7BC590F5E4}"/>
+    <hyperlink ref="C84" r:id="rId29" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{A7993C35-87EF-4D57-B068-CAEF63F66A3D}"/>
+    <hyperlink ref="C85" r:id="rId30" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{0403F257-6EB2-4A7B-A87D-067D1AB2D551}"/>
+    <hyperlink ref="C86" r:id="rId31" display="https://codeforces.com/problemset/problem/1/A" xr:uid="{6BCF84E3-A284-461A-86DE-53FDC72603A7}"/>
+    <hyperlink ref="C87" r:id="rId32" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{9F7A1ED6-D8B7-426A-9086-83607E4C549D}"/>
+    <hyperlink ref="C88" r:id="rId33" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{C5C1BBCF-9818-47A4-A233-B50FA9429233}"/>
+    <hyperlink ref="C89" r:id="rId34" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{224B315D-650D-49C7-897B-684432B22F89}"/>
+    <hyperlink ref="C90" r:id="rId35" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{82BCBC6B-9EEA-43C3-950D-B2267C954D25}"/>
+    <hyperlink ref="C91" r:id="rId36" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{DB40ECA1-59DD-4A7B-95A1-A9EB2BF1DE3F}"/>
+    <hyperlink ref="C92" r:id="rId37" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{B6DB19D7-35BC-4E8D-80B6-905A038CCDEF}"/>
+    <hyperlink ref="C93" r:id="rId38" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{6A7ECF2E-C033-476C-B046-4FDA56F795E4}"/>
+    <hyperlink ref="C94" r:id="rId39" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{3F662E96-0799-4FB3-85A6-8A40908F6D4B}"/>
+    <hyperlink ref="C95" r:id="rId40" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{838296D1-8F95-4A64-9633-4CCD40CBB151}"/>
+    <hyperlink ref="C96" r:id="rId41" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{7127B025-A0C4-4036-AAAE-1152AC06B63E}"/>
+    <hyperlink ref="C97" r:id="rId42" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{FFA75A85-BBF5-42B3-B599-9417443FBD93}"/>
+    <hyperlink ref="C98" r:id="rId43" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{498B3AC6-DED0-47D4-BEBF-E63ABA70E37D}"/>
+    <hyperlink ref="C99" r:id="rId44" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{AD351C80-0F1F-4D3E-BBD6-EC9D4FE819BB}"/>
+    <hyperlink ref="C100" r:id="rId45" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{18DEE90D-BDE3-49FB-817F-FFDE65FDCA04}"/>
+    <hyperlink ref="C101" r:id="rId46" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{D80F8E0E-72AD-466F-A8F1-5C06C34C7BD1}"/>
+    <hyperlink ref="C102" r:id="rId47" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{02157ABA-151C-4CF3-BE0F-5AA8640AF272}"/>
+    <hyperlink ref="C103" r:id="rId48" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{C6BD44CB-9E98-4D28-9BC1-164A6DC5AA93}"/>
+    <hyperlink ref="C104" r:id="rId49" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{5F4217AB-CB1F-4C58-952A-B2A3F6FE88EA}"/>
+    <hyperlink ref="C105" r:id="rId50" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{F1580A24-ABC6-405F-A44F-1F71FFE9DCDB}"/>
+    <hyperlink ref="C109" r:id="rId51" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{B7C58112-EE76-4593-9BA5-DCF1E3CD8AAE}"/>
+    <hyperlink ref="C110" r:id="rId52" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{00042F64-E8FA-423E-A177-24E7B6CEAB20}"/>
+    <hyperlink ref="C111" r:id="rId53" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{A8BDA395-7C69-4595-93FC-0282E0EFD4E3}"/>
+    <hyperlink ref="C112" r:id="rId54" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{D6D9789B-7968-41B9-B62A-C423BF937181}"/>
+    <hyperlink ref="C115" r:id="rId55" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{061F3928-7A09-48B4-8CBD-F5E169A283D4}"/>
+    <hyperlink ref="C116" r:id="rId56" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{7E02D882-E8DC-445B-8635-209825DCD6EE}"/>
+    <hyperlink ref="C117" r:id="rId57" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{D2E8D740-110B-4878-AD6C-1069825FA10B}"/>
+    <hyperlink ref="C118" r:id="rId58" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{F4261348-260E-4878-AE51-A1F0E1ED6298}"/>
+    <hyperlink ref="C121" r:id="rId59" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{B75C0EEC-FB79-4365-9EF9-4AAE5EC18F0F}"/>
+    <hyperlink ref="C122" r:id="rId60" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{0343B5CD-2F39-496E-92EF-FFE8FAF89D33}"/>
+    <hyperlink ref="C123" r:id="rId61" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{B9439D45-4675-42A0-82E7-91C154AC315C}"/>
+    <hyperlink ref="C124" r:id="rId62" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{AD186EAE-0FD8-4216-BF6F-5DE61E6C4F34}"/>
+    <hyperlink ref="C128" r:id="rId63" display="https://codeforces.com/contest/1370/problem/D" xr:uid="{A9BC2B41-3BCE-4E0C-8903-18F26C75DAD5}"/>
+    <hyperlink ref="C129" r:id="rId64" display="https://www.spoj.com/problems/TDPRIMES/" xr:uid="{9B8F96FB-D014-4380-AE5B-DCE44ABBAE96}"/>
+    <hyperlink ref="C130" r:id="rId65" display="https://www.spoj.com/problems/TDKPRIME/" xr:uid="{A7ABD4EB-BB21-4BC7-B624-06822DF33628}"/>
+    <hyperlink ref="C133" r:id="rId66" display="https://codeforces.com/contest/264/problem/B" xr:uid="{2765188F-D0D3-4B70-AD44-DBE5982EEB5A}"/>
+    <hyperlink ref="C134" r:id="rId67" display="https://codeforces.com/contest/735/problem/D" xr:uid="{D11505DB-7FE5-4015-AEF4-DA8106DD73E4}"/>
+    <hyperlink ref="C135" r:id="rId68" display="https://codeforces.com/contest/546/problem/D" xr:uid="{927CF4E1-9280-4408-93D0-DA69A9DAE8B0}"/>
+    <hyperlink ref="C136" r:id="rId69" display="https://codeforces.com/contest/222/problem/C" xr:uid="{F45A9FC6-52AA-4C68-9F76-8C19E7A13337}"/>
+    <hyperlink ref="C139" r:id="rId70" display="https://codeforces.com/problemset/problem/111/B" xr:uid="{BD609E2F-00A3-4A22-962F-E2D71C4A6D2E}"/>
+    <hyperlink ref="C140" r:id="rId71" display="https://codeforces.com/contest/1228/problem/C" xr:uid="{AA2E00E3-E993-4A6C-B471-4C76238D8063}"/>
+    <hyperlink ref="C141" r:id="rId72" display="https://codeforces.com/contest/1101/problem/D" xr:uid="{487DB7AF-AA15-4D4A-AB33-D91F5A4E1D86}"/>
+    <hyperlink ref="C145" r:id="rId73" display="https://codeforces.com/contest/1101/problem/D" xr:uid="{69594BDD-9D03-427E-9CB8-2E59A9111DD6}"/>
+    <hyperlink ref="C146" r:id="rId74" display="https://codeforces.com/problemset/problem/1594/B" xr:uid="{2872A028-6961-45D2-9F0A-7D669A2A65A2}"/>
+    <hyperlink ref="C147" r:id="rId75" display="https://codeforces.com/problemset/problem/1097/B" xr:uid="{F35596D7-C6C5-4E41-91E3-9F544BA72DE2}"/>
+    <hyperlink ref="C148" r:id="rId76" display="https://codeforces.com/contest/1602/problem/C" xr:uid="{8BFAC610-8856-44FA-9D80-167E4CFCC1CE}"/>
+    <hyperlink ref="C151" r:id="rId77" display="https://codeforces.com/problemset/problem/1095/C" xr:uid="{1052D211-0002-4ABD-BDBB-29D157AE6D1C}"/>
+    <hyperlink ref="C152" r:id="rId78" display="https://codeforces.com/problemset/problem/1494/B" xr:uid="{B5B8DCD0-E3C2-49B6-A69D-42DA41CB969E}"/>
+    <hyperlink ref="C153" r:id="rId79" display="https://codeforces.com/problemset/problem/1151/B" xr:uid="{CACD7565-91A6-4BD5-BC35-F3026B28F957}"/>
+    <hyperlink ref="C154" r:id="rId80" display="https://codeforces.com/problemset/problem/1225/C" xr:uid="{B717C621-3A69-4F5D-A616-853A14EDD8D5}"/>
+    <hyperlink ref="C157" r:id="rId81" display="https://codeforces.com/contest/1174/problem/D" xr:uid="{B41C2DE8-A239-40ED-A335-0C54ABB05668}"/>
+    <hyperlink ref="C158" r:id="rId82" display="https://codeforces.com/problemset/problem/1391/D" xr:uid="{6E115254-7035-4C9C-AA55-597B62FEC7AB}"/>
+    <hyperlink ref="C159" r:id="rId83" display="https://codeforces.com/problemset/problem/1491/D" xr:uid="{3AB9C53F-82AF-4E12-AD3D-076DE1F7BF63}"/>
+    <hyperlink ref="C163" r:id="rId84" display="https://codeforces.com/contest/343/problem/B" xr:uid="{60891248-7B8C-4617-B77F-ACFE7677F2E9}"/>
+    <hyperlink ref="C164" r:id="rId85" display="https://codeforces.com/contest/158/problem/C" xr:uid="{50E32397-6D45-4B01-987A-D19825EC78E2}"/>
+    <hyperlink ref="C165" r:id="rId86" display="https://codeforces.com/contest/5/problem/C" xr:uid="{8ABF07A6-A243-4672-BFEF-4CFED43512B1}"/>
+    <hyperlink ref="C168" r:id="rId87" display="https://codeforces.com/contest/359/problem/D" xr:uid="{D7E9C3C4-E2F0-4A30-825F-81AE50FE6EB1}"/>
+    <hyperlink ref="C169" r:id="rId88" display="https://codeforces.com/contest/1092/problem/D1" xr:uid="{EA699C53-903F-45EA-941F-2A8DB25652A0}"/>
+    <hyperlink ref="C170" r:id="rId89" display="https://codeforces.com/contest/1313/problem/C2" xr:uid="{91C3E5D5-7199-4582-8613-1C5660DDE26A}"/>
+    <hyperlink ref="C171" r:id="rId90" display="https://codeforces.com/contest/1515/problem/C" xr:uid="{9600B657-7CED-4AEF-9997-3E58B777B4FC}"/>
+    <hyperlink ref="C174" r:id="rId91" display="https://codeforces.com/contest/319/problem/B" xr:uid="{63920447-6665-42B4-9750-0A8A96E20038}"/>
+    <hyperlink ref="C175" r:id="rId92" display="https://codeforces.com/contest/487/problem/B" xr:uid="{2B512440-7FD9-41E9-9F0A-F5847F1CB9CC}"/>
+    <hyperlink ref="C176" r:id="rId93" display="https://codeforces.com/contest/1092/problem/D2" xr:uid="{47843149-CAA3-453B-84F6-C5990E504EB9}"/>
+    <hyperlink ref="C177" r:id="rId94" display="https://codeforces.com/contest/1156/problem/E" xr:uid="{10AD5C70-4E84-4C2C-A8DA-32A9D35DBADB}"/>
+    <hyperlink ref="C178" r:id="rId95" display="https://codeforces.com/contest/911/problem/E" xr:uid="{8604D6DD-DE06-4185-9618-1AB590B54309}"/>
+    <hyperlink ref="C179" r:id="rId96" display="https://codeforces.com/contest/507/problem/E?locale=en" xr:uid="{C050C26C-B665-41F3-957A-454CCEB3FFE8}"/>
+    <hyperlink ref="C183" r:id="rId97" display="https://codeforces.com/problemset/problem/271/D" xr:uid="{44A3B5D5-C6D4-4399-9FC0-56461D4260AC}"/>
+    <hyperlink ref="C184" r:id="rId98" display="https://codeforces.com/contest/1326/problem/D2" xr:uid="{715E2A38-958E-4788-9451-A3ABCFB20DE6}"/>
+    <hyperlink ref="C185" r:id="rId99" display="https://codeforces.com/contest/514/problem/C" xr:uid="{94FDA7D8-67B3-4DD3-810D-19A86C4B1C17}"/>
+    <hyperlink ref="C186" r:id="rId100" display="https://codeforces.com/contest/7/problem/D" xr:uid="{6ACAA64C-0929-4476-99D0-CD08CC2E2414}"/>
+    <hyperlink ref="C187" r:id="rId101" display="https://codeforces.com/contest/514/problem/C" xr:uid="{6701AE01-6DFC-4B04-9FE8-A33268FE31C1}"/>
+    <hyperlink ref="C188" r:id="rId102" display="https://codeforces.com/contest/633/problem/C" xr:uid="{00B2BD2E-717A-4E06-819B-C22FAC98720A}"/>
+    <hyperlink ref="C191" r:id="rId103" display="https://codeforces.com/contest/1016/problem/B" xr:uid="{4C80B6E8-2C12-425A-8ED9-1707185AF4B7}"/>
+    <hyperlink ref="C192" r:id="rId104" display="https://codeforces.com/contest/471/problem/D" xr:uid="{9C5B0546-C5C6-4FA5-8AE7-2D9B6E0D4D96}"/>
+    <hyperlink ref="C193" r:id="rId105" display="https://codeforces.com/problemset/problem/126/B" xr:uid="{F87A64E5-3538-419C-9A0C-57FB1FFE7C4B}"/>
+    <hyperlink ref="C194" r:id="rId106" display="https://codeforces.com/contest/471/problem/D" xr:uid="{A0AC9302-3D99-44D2-9354-D83D66F3CE2A}"/>
+    <hyperlink ref="C195" r:id="rId107" display="https://codeforces.com/contest/1138/problem/D" xr:uid="{3475B623-6F0C-46A1-8FCD-93EF1DD7BEB8}"/>
+    <hyperlink ref="C196" r:id="rId108" display="https://codeforces.com/contest/126/problem/B" xr:uid="{71E8E9B9-F0E6-4A7D-B28B-238F5C6E3377}"/>
+    <hyperlink ref="C197" r:id="rId109" display="https://codeforces.com/contest/432/problem/D" xr:uid="{EF947049-8495-4B21-995C-8EC9A2D81E51}"/>
+    <hyperlink ref="C198" r:id="rId110" display="https://codeforces.com/contest/1537/problem/E2" xr:uid="{18239E1F-8DBB-4DCB-8748-9E74DE91E313}"/>
+    <hyperlink ref="C201" r:id="rId111" display="https://www.spoj.com/problems/NUMOFPAL/" xr:uid="{323E93AB-1832-45B5-BF32-41914A1391DA}"/>
+    <hyperlink ref="C202" r:id="rId112" display="https://www.spoj.com/problems/LPS/" xr:uid="{9B4DB6E4-6F3B-4EEA-8222-DAE9C031EE19}"/>
+    <hyperlink ref="C203" r:id="rId113" display="https://www.spoj.com/problems/MSUBSTR/" xr:uid="{0DA58C82-02FD-40CC-808D-2F89C48EDA0D}"/>
+    <hyperlink ref="C204" r:id="rId114" display="https://www.spoj.com/problems/EPALIN/" xr:uid="{9051C92C-A2C5-4EAB-8774-DCCAFA384F99}"/>
+    <hyperlink ref="C205" r:id="rId115" display="https://codeforces.com/contest/1080/problem/E" xr:uid="{1A22C955-CBCB-402C-BA4C-05DFDBBC3E0D}"/>
+    <hyperlink ref="C208" r:id="rId116" display="https://codeforces.com/problemset/problem/1006/F" xr:uid="{5DB7211F-15E1-4360-95DA-35051BDFB59A}"/>
+    <hyperlink ref="C212" r:id="rId117" display="https://cses.fi/problemset/task/1674" xr:uid="{7FFB5365-1980-470D-894F-4201C72C5B8B}"/>
+    <hyperlink ref="C213" r:id="rId118" display="https://cses.fi/problemset/task/1130" xr:uid="{FF3A5286-BDE1-4F90-A26B-CC3D774CDED5}"/>
+    <hyperlink ref="C214" r:id="rId119" display="https://codeforces.com/gym/102694/problem/A" xr:uid="{9380042F-2697-4EBF-A306-633B58E2659E}"/>
+    <hyperlink ref="C215" r:id="rId120" display="https://codeforces.com/gym/102694/problem/B" xr:uid="{DD89A320-B792-4BC4-BEA4-C93936F7BD2E}"/>
+    <hyperlink ref="C218" r:id="rId121" display="https://codeforces.com/gym/102694/problem/A" xr:uid="{ED37F328-7516-4CF5-9CD5-16B6914F95C6}"/>
+    <hyperlink ref="C219" r:id="rId122" display="https://cses.fi/problemset/task/1133" xr:uid="{DDB64992-5418-42DE-8679-F1618F85EAD8}"/>
+    <hyperlink ref="C220" r:id="rId123" display="https://codeforces.com/contest/1294/problem/F" xr:uid="{A149CC9E-6043-4EA3-A74D-823754D9461A}"/>
+    <hyperlink ref="C225" r:id="rId124" display="https://codeforces.com/gym/102694/problem/C" xr:uid="{E7F43E13-BFC6-4B09-86D9-FB2267C1BECA}"/>
+    <hyperlink ref="C226" r:id="rId125" display="https://codeforces.com/gym/102694/problem/D" xr:uid="{F714D048-6AAF-4EA0-BA78-D650D77FBCFF}"/>
+    <hyperlink ref="C230" r:id="rId126" display="https://codeforces.com/contest/1328/problem/E" xr:uid="{76E17511-72BA-49E3-9250-D5784BEC974B}"/>
+    <hyperlink ref="C231" r:id="rId127" display="https://codeforces.com/contest/1304/problem/E" xr:uid="{FF4FA1F2-B40E-4FA3-A656-2B30BE7572D8}"/>
+    <hyperlink ref="C232" r:id="rId128" display="https://codeforces.com/contest/208/problem/E" xr:uid="{4A4A7A4C-6683-4A5A-9961-6EDD4B58DC98}"/>
+    <hyperlink ref="C233" r:id="rId129" display="https://codeforces.com/contest/191/problem/C" xr:uid="{3FBD5886-F9ED-46A9-B006-D1DC6D17C33F}"/>
+    <hyperlink ref="C237" r:id="rId130" display="https://codeforces.com/contest/519/problem/E" xr:uid="{CED2A27E-BE1F-403F-8128-A51802531F2E}"/>
+    <hyperlink ref="C238" r:id="rId131" display="https://codeforces.com/contest/587/problem/C" xr:uid="{68F8782D-0553-417F-9F79-6296E70263B7}"/>
+    <hyperlink ref="C239" r:id="rId132" display="https://codeforces.com/contest/609/problem/E" xr:uid="{A69F627D-8B97-415C-A36E-22FFEE8C2F38}"/>
+    <hyperlink ref="C240" r:id="rId133" display="https://codeforces.com/contest/466/problem/E" xr:uid="{A9DC7A38-4FFF-43E6-97A7-836F74BE5F87}"/>
+    <hyperlink ref="C244" r:id="rId134" display="https://codeforces.com/gym/102694/problem/E" xr:uid="{2356EAA5-E8F4-4F65-BDF1-53CD27FE09D2}"/>
+    <hyperlink ref="C245" r:id="rId135" display="https://codeforces.com/gym/102694/problem/F" xr:uid="{23220DCA-2714-4BF3-96A5-C116E94A2732}"/>
+    <hyperlink ref="C249" r:id="rId136" display="https://codeforces.com/problemset/problem/520/B" xr:uid="{03CE039F-08B2-4E70-96F8-4BBE007E8F85}"/>
+    <hyperlink ref="C250" r:id="rId137" display="https://codeforces.com/problemset/problem/115/A" xr:uid="{07763546-702A-488F-B361-FF5B07E1B66B}"/>
+    <hyperlink ref="C251" r:id="rId138" display="https://codeforces.com/problemset/problem/580/C" xr:uid="{BDD811C1-5E29-47D3-AAFF-7DDA240C534D}"/>
+    <hyperlink ref="C252" r:id="rId139" display="https://codeforces.com/problemset/problem/977/E" xr:uid="{8DBACEA7-048B-43A2-94BC-E04BEA8F9451}"/>
+    <hyperlink ref="C253" r:id="rId140" display="https://codeforces.com/contest/1144/problem/F" xr:uid="{9FE16E68-8FF3-460E-92B7-DAB7B208FF7C}"/>
+    <hyperlink ref="C254" r:id="rId141" display="https://codeforces.com/contest/510/problem/C" xr:uid="{33A4D3B2-E777-44B9-B84E-459A2ECECACA}"/>
+    <hyperlink ref="C255" r:id="rId142" display="https://codeforces.com/contest/20/problem/C" xr:uid="{D127B550-ED72-4E18-A082-F576D3C4BA4E}"/>
+    <hyperlink ref="C256" r:id="rId143" display="https://codeforces.com/problemset/problem/475/B" xr:uid="{70DCAABE-9F1B-4729-86FF-8B1CB3AF8E26}"/>
+    <hyperlink ref="C259" r:id="rId144" display="https://codeforces.com/contest/986/problem/A" xr:uid="{D02ECCA4-F730-448F-B6F1-939563C28D14}"/>
+    <hyperlink ref="C260" r:id="rId145" display="https://codeforces.com/contest/242/problem/C" xr:uid="{FD61155A-7608-4817-A8B3-3F717CFB1439}"/>
+    <hyperlink ref="C261" r:id="rId146" display="https://codeforces.com/contest/1345/problem/D" xr:uid="{384CC8F1-B40A-489B-AC88-53B0429E03BA}"/>
+    <hyperlink ref="C262" r:id="rId147" display="https://codeforces.com/contest/229/problem/B" xr:uid="{1FD52FED-045C-409F-8E53-06D049A34D17}"/>
+    <hyperlink ref="C263" r:id="rId148" display="https://codeforces.com/contest/1385/problem/E" xr:uid="{EE15E94D-9D36-4C47-B417-1675FA127C6B}"/>
+    <hyperlink ref="C264" r:id="rId149" display="https://codeforces.com/contest/295/problem/B" xr:uid="{0DC2B729-DC20-4842-A7A7-719CFDB205D7}"/>
+    <hyperlink ref="C265" r:id="rId150" display="https://codeforces.com/contest/1213/problem/F" xr:uid="{13C08E4F-BC6F-4401-84F4-30EE7AAE25AE}"/>
+    <hyperlink ref="C266" r:id="rId151" display="https://codeforces.com/contest/1343/problem/E" xr:uid="{F05DEB4E-A305-474F-9DCB-E47B747BC2AF}"/>
+    <hyperlink ref="C267" r:id="rId152" display="https://codeforces.com/contest/1296/problem/E1" xr:uid="{6380A587-6E91-4CA2-9898-0CF85961D8DF}"/>
+    <hyperlink ref="C270" r:id="rId153" display="https://codeforces.com/contest/1573/problem/C" xr:uid="{172ADCDE-5E1B-46A8-A8CD-A1F3A6C4598A}"/>
+    <hyperlink ref="C271" r:id="rId154" display="https://codeforces.com/contest/1547/problem/G" xr:uid="{68D336F3-BAAD-4EBC-83E5-000235EEE4AF}"/>
+    <hyperlink ref="C272" r:id="rId155" display="https://codeforces.com/contest/229/problem/B" xr:uid="{35855A60-5E9C-4A54-A606-899BDB16A77F}"/>
+    <hyperlink ref="C273" r:id="rId156" display="https://codeforces.com/contest/400/problem/D" xr:uid="{72DC67D7-EAEE-4D38-B99F-38FE9CE0C123}"/>
+    <hyperlink ref="C274" r:id="rId157" display="https://codeforces.com/contest/178/problem/B3" xr:uid="{7FF1E0ED-2F07-4EB3-AD0E-59EDAC055801}"/>
+    <hyperlink ref="C277" r:id="rId158" display="https://codeforces.com/problemset/problem/185/A" xr:uid="{903674CA-0720-4A19-B92F-8AD6DAED854A}"/>
+    <hyperlink ref="C278" r:id="rId159" display="https://codeforces.com/contest/1117/problem/D" xr:uid="{07824635-BA83-4FE1-8CC3-9A6D12288666}"/>
+    <hyperlink ref="C279" r:id="rId160" display="https://codeforces.com/contest/582/problem/B" xr:uid="{10109640-8108-443F-8620-B847F104CB13}"/>
+    <hyperlink ref="C280" r:id="rId161" display="https://codeforces.com/contest/222/problem/E" xr:uid="{D5085D74-6CFD-48DF-AE27-632B639EF9D9}"/>
+    <hyperlink ref="C281" r:id="rId162" display="https://codeforces.com/contest/621/problem/E" xr:uid="{ED16D8F6-66AA-4378-90B1-8A51D3F534FF}"/>
+    <hyperlink ref="C282" r:id="rId163" display="https://codeforces.com/contest/1182/problem/E" xr:uid="{5CB6B1DD-4D4C-4985-9FE7-037910CD3270}"/>
+    <hyperlink ref="C285" r:id="rId164" display="https://codeforces.com/contest/706/problem/D" xr:uid="{48686123-F8FC-43B1-BE84-27098373DAC9}"/>
+    <hyperlink ref="C286" r:id="rId165" display="https://codeforces.com/contest/948/problem/D" xr:uid="{E8923895-166D-4A1F-BB8D-46590BA4DBD6}"/>
+    <hyperlink ref="C287" r:id="rId166" display="https://codeforces.com/contest/665/problem/E" xr:uid="{D7885557-77BE-4E04-990F-C82385E08D44}"/>
+    <hyperlink ref="C288" r:id="rId167" display="https://codeforces.com/contest/1285/problem/D" xr:uid="{32B74896-AD74-486E-A0FF-95C9A142ECB1}"/>
+    <hyperlink ref="C289" r:id="rId168" display="https://codeforces.com/contest/858/problem/D" xr:uid="{8D47675A-9A4E-4455-9BCA-50A06F323245}"/>
+    <hyperlink ref="C290" r:id="rId169" display="https://codeforces.com/contest/455/problem/B" xr:uid="{E0C4AEA9-6B4E-494F-B268-29067F3A3EC8}"/>
+    <hyperlink ref="C291" r:id="rId170" display="https://codeforces.com/contest/113/problem/B" xr:uid="{ED89D802-CE14-4461-A520-8BB9BD8BE1AA}"/>
+    <hyperlink ref="C292" r:id="rId171" display="https://codeforces.com/contest/282/problem/E" xr:uid="{EA845F39-5B96-4069-8B21-983DBC58DF14}"/>
+    <hyperlink ref="C296" r:id="rId172" display="https://codeforces.com/problemset/problem/702/A" xr:uid="{E9CB2DE9-88D2-48C8-8177-E4B35AE538A3}"/>
+    <hyperlink ref="C297" r:id="rId173" display="https://codeforces.com/problemset/problem/894/A" xr:uid="{45DD1ECF-6BF4-4EB1-8EB4-A127D524D50A}"/>
+    <hyperlink ref="C298" r:id="rId174" display="https://codeforces.com/problemset/problem/1501/B" xr:uid="{4FBEEB1D-F34E-4C6E-9591-1FA9D23C1A7E}"/>
+    <hyperlink ref="C299" r:id="rId175" display="https://codeforces.com/problemset/problem/1469/B" xr:uid="{435C14CC-3600-4444-BB39-C07F61F30FB8}"/>
+    <hyperlink ref="C300" r:id="rId176" display="https://codeforces.com/problemset/problem/363/B" xr:uid="{BA1030A2-0B68-42AE-AB50-216C4203E3E9}"/>
+    <hyperlink ref="C301" r:id="rId177" display="https://codeforces.com/problemset/problem/313/B" xr:uid="{BC5B1306-257D-44A1-8624-5505A9EB40C7}"/>
+    <hyperlink ref="C302" r:id="rId178" display="https://codeforces.com/problemset/problem/327/A" xr:uid="{5BD0C670-1BFF-49BF-A382-3E757D216AAD}"/>
+    <hyperlink ref="C303" r:id="rId179" display="https://codeforces.com/problemset/problem/961/B" xr:uid="{8A379A09-06DF-4F8D-8DD8-5C5124AB00D7}"/>
+    <hyperlink ref="C304" r:id="rId180" display="https://codeforces.com/problemset/problem/522/A" xr:uid="{FF5DD54E-F619-46DF-B65B-A27FAD9EFA1F}"/>
+    <hyperlink ref="C305" r:id="rId181" display="https://codeforces.com/problemset/problem/1042/B" xr:uid="{1185A058-2C9D-4BA9-A28F-FB887BFEE948}"/>
+    <hyperlink ref="C306" r:id="rId182" display="https://codeforces.com/problemset/problem/189/A" xr:uid="{4D886BB8-3373-44B4-B08A-E3F5CAA5264C}"/>
+    <hyperlink ref="C307" r:id="rId183" display="https://codeforces.com/problemset/problem/1420/C1" xr:uid="{CC56CF98-4333-4B42-8952-08D42456AEF4}"/>
+    <hyperlink ref="C308" r:id="rId184" display="https://codeforces.com/problemset/problem/414/B" xr:uid="{BA3CB3F1-8EF6-47D4-A88E-63C6AEA83989}"/>
+    <hyperlink ref="C309" r:id="rId185" display="https://codeforces.com/problemset/problem/1195/C" xr:uid="{12D783EC-8F92-4786-ABCF-CCC4C791CC68}"/>
+    <hyperlink ref="C310" r:id="rId186" display="https://codeforces.com/problemset/problem/1350/B" xr:uid="{3F0BEA35-B386-4831-9BAF-0EAEA90475CA}"/>
+    <hyperlink ref="C313" r:id="rId187" display="https://codeforces.com/contest/505/problem/C" xr:uid="{A34BB500-070D-46A4-82C9-18161C0DD247}"/>
+    <hyperlink ref="C314" r:id="rId188" display="https://codeforces.com/contest/577/problem/B" xr:uid="{C84FF700-349E-48AC-B275-E3F3056D2F3C}"/>
+    <hyperlink ref="C315" r:id="rId189" display="https://codeforces.com/contest/204/problem/A" xr:uid="{91186E77-D348-48B6-8451-4FFC525AEC89}"/>
+    <hyperlink ref="C316" r:id="rId190" display="https://codeforces.com/contest/448/problem/C" xr:uid="{F22C51E8-1F52-47C6-BBD7-ECD4C3D616B6}"/>
+    <hyperlink ref="C317" r:id="rId191" display="https://codeforces.com/contest/479/problem/E" xr:uid="{28718124-3B57-4951-9AAA-E47240184D16}"/>
+    <hyperlink ref="C318" r:id="rId192" display="https://codeforces.com/contest/401/problem/D" xr:uid="{8A721A57-1986-457A-8021-87A60BC9E699}"/>
+    <hyperlink ref="C319" r:id="rId193" display="https://codeforces.com/contest/777/problem/E" xr:uid="{F86235DE-3239-4B04-A0FD-C5AC87EAE1D4}"/>
+    <hyperlink ref="C320" r:id="rId194" display="https://codeforces.com/contest/1036/problem/C" xr:uid="{ABFBFFD1-073A-401C-8C5D-97E718137EBF}"/>
+    <hyperlink ref="C321" r:id="rId195" display="https://codeforces.com/contest/219/problem/D" xr:uid="{FE90156B-2AA2-40BA-AFEB-83DADB93039D}"/>
+    <hyperlink ref="C322" r:id="rId196" display="https://codeforces.com/contest/337/problem/D" xr:uid="{28820F82-1B1E-47ED-87E2-A974AFF3E684}"/>
+    <hyperlink ref="C325" r:id="rId197" display="https://codeforces.com/contest/165/problem/E" xr:uid="{F68F6AFD-FA8C-4D3A-A69B-42B31D25653D}"/>
+    <hyperlink ref="C326" r:id="rId198" display="https://codeforces.com/contest/687/problem/C" xr:uid="{3FA5A113-AFCF-441C-BD48-A1CF8C9DDB26}"/>
+    <hyperlink ref="C327" r:id="rId199" display="https://codeforces.com/contest/1132/problem/F" xr:uid="{F4643E28-4C15-45FC-A72A-508D9CE7C22F}"/>
+    <hyperlink ref="C328" r:id="rId200" display="https://codeforces.com/contest/1253/problem/E" xr:uid="{0CA1D004-898E-4052-BCB3-54F2911052DA}"/>
+    <hyperlink ref="C329" r:id="rId201" display="https://codeforces.com/contest/1216/problem/F" xr:uid="{7E93F84E-E741-4BBC-9E99-025DE5BFBD25}"/>
+    <hyperlink ref="C330" r:id="rId202" display="https://codeforces.com/contest/461/problem/B" xr:uid="{2DAB43C0-BC57-4F91-9E77-E0838FA70381}"/>
+    <hyperlink ref="C331" r:id="rId203" display="https://codeforces.com/contest/319/problem/C" xr:uid="{AEB06620-C1E7-4211-B3D4-B60C1779E691}"/>
+    <hyperlink ref="C332" r:id="rId204" display="https://codeforces.com/contest/1083/problem/E" xr:uid="{7F0B980C-F0C8-43DD-8BA6-C856B3205FD7}"/>
+    <hyperlink ref="C333" r:id="rId205" display="https://codeforces.com/contest/507/problem/D" xr:uid="{B41A95E1-F69F-4364-8ACE-0144A1D1C644}"/>
+    <hyperlink ref="C334" r:id="rId206" display="https://codeforces.com/contest/540/problem/D" xr:uid="{208ADE34-2713-4257-80F8-DBB8D5F837B8}"/>
+    <hyperlink ref="C338" r:id="rId207" display="https://codeforces.com/problemset/problem/1534/C" xr:uid="{C702161A-8805-47E1-8225-74639226D8E2}"/>
+    <hyperlink ref="C339" r:id="rId208" display="https://codeforces.com/problemset/problem/217/A" xr:uid="{EC12BDBD-4FFD-49A1-83E6-BFBCBCB07A4B}"/>
+    <hyperlink ref="C340" r:id="rId209" display="https://codeforces.com/contest/277/problem/A" xr:uid="{DCBF8D08-1CCB-49AB-BB96-C5694048DEE5}"/>
+    <hyperlink ref="C343" r:id="rId210" display="https://codeforces.com/contest/884/problem/C" xr:uid="{689CFB1A-E1C1-4E26-B3E3-418CAA5A6D0E}"/>
+    <hyperlink ref="C344" r:id="rId211" display="https://codeforces.com/contest/1332/problem/C" xr:uid="{EE66C364-1C95-4220-B361-C8FF433F9404}"/>
+    <hyperlink ref="C345" r:id="rId212" display="https://codeforces.com/contest/455/problem/C" xr:uid="{634B5492-0C59-41F6-990B-84E1DC600A37}"/>
+    <hyperlink ref="C348" r:id="rId213" display="https://codeforces.com/contest/1156/problem/D" xr:uid="{6EF110B4-33FA-4F45-8FF2-9F13DABF1BB4}"/>
+    <hyperlink ref="C349" r:id="rId214" display="https://codeforces.com/contest/1213/problem/G" xr:uid="{A56E2B52-F95B-4ECA-8659-EDA02DF7ABD3}"/>
+    <hyperlink ref="C350" r:id="rId215" display="https://codeforces.com/problemset/problem/1494/D" xr:uid="{6F2E5012-EEAE-49ED-A2F3-FE16C3ECB4D6}"/>
+    <hyperlink ref="C351" r:id="rId216" display="https://codeforces.com/problemset/problem/455/C" xr:uid="{A267F2D5-B666-44E0-B422-78D2B4831B43}"/>
+    <hyperlink ref="C354" r:id="rId217" display="https://codeforces.com/problemset/problem/455/C" xr:uid="{BDB565D4-77CE-4F3F-8B12-B5D154D3A474}"/>
+    <hyperlink ref="C355" r:id="rId218" display="https://codeforces.com/contest/617/problem/E" xr:uid="{D9653234-537C-439C-A89E-6AAF59570145}"/>
+    <hyperlink ref="C356" r:id="rId219" display="https://codeforces.com/contest/220/problem/B" xr:uid="{BE689AA3-70EE-4631-9831-178D5A6365A1}"/>
+    <hyperlink ref="C357" r:id="rId220" display="https://codeforces.com/contest/1514/problem/D" xr:uid="{8D3CA309-A854-42B3-9C84-D1AC96176234}"/>
+    <hyperlink ref="C358" r:id="rId221" display="https://codeforces.com/contest/375/problem/D" xr:uid="{FF786C16-8978-4A96-863F-C1D3A1D33F0E}"/>
+    <hyperlink ref="C359" r:id="rId222" display="https://codeforces.com/contest/242/problem/E" xr:uid="{4F1239AB-D143-4DBA-8F2B-B80B8888794A}"/>
+    <hyperlink ref="C362" r:id="rId223" display="https://codeforces.com/contest/61/problem/E" xr:uid="{8EF670D2-1707-410B-AAA1-312462EEA484}"/>
+    <hyperlink ref="C363" r:id="rId224" display="https://codeforces.com/contest/1311/problem/F" xr:uid="{FF0F8182-D5D0-4195-93D3-3AF36451C3A2}"/>
+    <hyperlink ref="C364" r:id="rId225" display="https://codeforces.com/contest/283/problem/A" xr:uid="{8243D1D2-CA64-4DAC-B265-4AA1A2412FE2}"/>
+    <hyperlink ref="C365" r:id="rId226" display="https://codeforces.com/contest/459/problem/D" xr:uid="{47EA03F6-03CF-4D3B-91AB-75C6C77DF2A0}"/>
+    <hyperlink ref="C366" r:id="rId227" display="https://codeforces.com/contest/340/problem/D" xr:uid="{187067DD-D539-4AFB-A27C-FF3B00381C73}"/>
+    <hyperlink ref="C367" r:id="rId228" display="https://codeforces.com/contest/1076/problem/E" xr:uid="{D5C6E09A-F164-4AF7-9870-53165C652E17}"/>
+    <hyperlink ref="C368" r:id="rId229" display="https://codeforces.com/contest/1354/problem/D" xr:uid="{2FCBF469-5C35-4CDD-8CF1-D7214D125C9A}"/>
+    <hyperlink ref="C369" r:id="rId230" display="https://codeforces.com/contest/1405/problem/E" xr:uid="{E76E6E9E-7419-4F9F-8210-26E2ED06CFF2}"/>
+    <hyperlink ref="C370" r:id="rId231" display="https://codeforces.com/contest/383/problem/C" xr:uid="{23843970-D3D1-4ED0-B16A-D93BC0596B1E}"/>
+    <hyperlink ref="C371" r:id="rId232" display="https://codeforces.com/contest/1526/problem/D" xr:uid="{D6B904D3-2D5E-46BF-99AF-F1A9BD57E273}"/>
+    <hyperlink ref="C372" r:id="rId233" display="https://codeforces.com/contest/276/problem/E" xr:uid="{3C8EF79E-8952-41B4-98D3-0EED34544C26}"/>
+    <hyperlink ref="C373" r:id="rId234" display="https://codeforces.com/contest/375/problem/D" xr:uid="{018C5B9B-9D8F-4A87-A015-C6AF61D58DB4}"/>
+    <hyperlink ref="C376" r:id="rId235" display="https://codeforces.com/contest/339/problem/D" xr:uid="{007FBF91-F09C-4404-BA7A-E454466AA24D}"/>
+    <hyperlink ref="C377" r:id="rId236" display="https://codeforces.com/contest/914/problem/D" xr:uid="{4A87C3E9-AA02-4EB4-BFE1-D49DB7F24C90}"/>
+    <hyperlink ref="C378" r:id="rId237" display="https://codeforces.com/contest/459/problem/D" xr:uid="{DDCB0CEE-BE07-449A-A01A-AD6D27FB0D33}"/>
+    <hyperlink ref="C379" r:id="rId238" display="https://codeforces.com/contest/61/problem/E" xr:uid="{22095C40-BB89-4376-A758-66AADF897596}"/>
+    <hyperlink ref="C380" r:id="rId239" display="https://codeforces.com/contest/380/problem/C" xr:uid="{E33C2986-BD5E-469C-866B-C7A1155D9185}"/>
+    <hyperlink ref="C381" r:id="rId240" display="https://codeforces.com/contest/474/problem/F" xr:uid="{ADB50F96-7C3A-416C-941B-F281011EB73F}"/>
+    <hyperlink ref="C382" r:id="rId241" display="https://codeforces.com/contest/1237/problem/D" xr:uid="{CA5FB483-8226-41F3-A807-92897DD0AF68}"/>
+    <hyperlink ref="C383" r:id="rId242" display="https://codeforces.com/contest/292/problem/E" xr:uid="{8014A4D0-2FBB-43E7-8E8B-C439C3F885DB}"/>
+    <hyperlink ref="C384" r:id="rId243" display="https://codeforces.com/contest/482/problem/B" xr:uid="{D7001310-52CF-4448-877A-2D82FA553FDB}"/>
+    <hyperlink ref="C385" r:id="rId244" display="https://codeforces.com/contest/1187/problem/D" xr:uid="{A82BD182-2528-4C02-86AE-8506D48094C9}"/>
+    <hyperlink ref="C386" r:id="rId245" display="https://codeforces.com/contest/920/problem/F" xr:uid="{E0E6F155-2F47-4079-A6BE-724897B295EF}"/>
+    <hyperlink ref="C387" r:id="rId246" display="https://codeforces.com/contest/1535/problem/D?locale=en" xr:uid="{BFF507B3-ABFC-412A-8855-FD1D9DAB4404}"/>
+    <hyperlink ref="C388" r:id="rId247" display="https://codeforces.com/contest/438/problem/D?locale=en" xr:uid="{D7D8F26B-28F7-4421-B505-1A50D99C7966}"/>
+    <hyperlink ref="C389" r:id="rId248" display="https://codeforces.com/contest/1556/problem/E" xr:uid="{63AE4160-9A44-45DE-83ED-1C1854964B2B}"/>
+    <hyperlink ref="C390" r:id="rId249" display="https://codeforces.com/contest/1567/problem/E" xr:uid="{066550AD-B9BE-4EC9-B0D3-3C7C7F90F7A1}"/>
+    <hyperlink ref="C393" r:id="rId250" display="https://codeforces.com/contest/52/problem/C" xr:uid="{F7A36424-5B0B-4295-B7AE-41BCAF57DE00}"/>
+    <hyperlink ref="C394" r:id="rId251" display="https://codeforces.com/contest/1023/problem/D" xr:uid="{28BD986E-8622-41B9-A104-58A55C28DDB9}"/>
+    <hyperlink ref="C395" r:id="rId252" display="https://codeforces.com/contest/242/problem/E" xr:uid="{1CA2E82E-F835-4825-A47A-E7A6E0A885CB}"/>
+    <hyperlink ref="C396" r:id="rId253" display="https://codeforces.com/contest/1557/problem/D" xr:uid="{9955F7AD-C0EF-48B4-A08E-FB979B0B1D8C}"/>
+    <hyperlink ref="C397" r:id="rId254" display="https://codeforces.com/contest/145/problem/E" xr:uid="{C5723FFD-146D-497B-97B4-9222F7F8140F}"/>
+    <hyperlink ref="C398" r:id="rId255" display="https://codeforces.com/contest/777/problem/E" xr:uid="{5EF62371-CBD1-4478-ADB5-7390ACE0BE95}"/>
+    <hyperlink ref="C4" r:id="rId256" display="https://codeforces.com/problemset/problem/282/A" xr:uid="{887FDAA3-AA07-4820-AFE1-5A181DC3FC02}"/>
+    <hyperlink ref="C5" r:id="rId257" display="https://codeforces.com/contest/514/problem/A" xr:uid="{51939345-F26A-4695-A578-3EFB06101B88}"/>
+    <hyperlink ref="C6" r:id="rId258" display="https://codeforces.com/problemset/problem/263/A" xr:uid="{E42EC0DB-E227-42E4-A963-3E2C3B3AB2A6}"/>
+    <hyperlink ref="C7" r:id="rId259" display="https://codeforces.com/problemset/problem/151/A" xr:uid="{463D9BD6-F65C-4792-96DF-ED99DEF5E174}"/>
+    <hyperlink ref="C8" r:id="rId260" display="https://codeforces.com/problemset/problem/723/A" xr:uid="{53924ED1-AFFB-4DC2-A466-6002FE456EA4}"/>
+    <hyperlink ref="C9" r:id="rId261" display="https://codeforces.com/problemset/problem/1352/A" xr:uid="{D469046F-522F-43BF-9297-0B1BCB48ECBD}"/>
+    <hyperlink ref="C10" r:id="rId262" display="https://codeforces.com/problemset/problem/510/A" xr:uid="{EA453CAB-0F5F-45CB-BF23-9FCFDF1456FD}"/>
+    <hyperlink ref="C11" r:id="rId263" display="https://codeforces.com/problemset/problem/785/A" xr:uid="{E7B69095-AA58-426E-B8C2-E846274C09CA}"/>
+    <hyperlink ref="C12" r:id="rId264" display="https://codeforces.com/problemset/problem/144/A" xr:uid="{E1DD219F-34ED-430A-89A3-91865C51288A}"/>
+    <hyperlink ref="C13" r:id="rId265" display="https://codeforces.com/problemset/problem/1030/A" xr:uid="{11529EF0-E61D-472B-B739-ABAFE31954AB}"/>
+    <hyperlink ref="C14" r:id="rId266" display="https://codeforces.com/problemset/problem/136/A" xr:uid="{C63150AF-B292-4FB6-876F-1327CC9A4D6E}"/>
+    <hyperlink ref="C15" r:id="rId267" display="https://codeforces.com/problemset/problem/110/A" xr:uid="{87488356-C265-4C61-AC31-C36A5281BD0E}"/>
+    <hyperlink ref="C16" r:id="rId268" display="https://codeforces.com/problemset/problem/116/A" xr:uid="{B7588F4E-1CBE-4537-81ED-D7C188887B16}"/>
+    <hyperlink ref="C17" r:id="rId269" display="https://codeforces.com/problemset/problem/977/A" xr:uid="{27B7CF3B-CB06-43CF-9469-A0D3CAC27A4C}"/>
+    <hyperlink ref="C18" r:id="rId270" display="https://codeforces.com/problemset/problem/546/A" xr:uid="{4AF24EC5-2F25-47B8-B166-BF6A14AA92BB}"/>
+    <hyperlink ref="C19" r:id="rId271" display="https://codeforces.com/problemset/problem/791/A" xr:uid="{0C780444-D411-4D8A-A1C8-D6A2C05F6155}"/>
+    <hyperlink ref="C20" r:id="rId272" display="https://codeforces.com/problemset/problem/236/A" xr:uid="{4A1465BF-5341-429A-9E61-658D5F587A3B}"/>
+    <hyperlink ref="C21" r:id="rId273" display="https://codeforces.com/problemset/problem/281/A" xr:uid="{84EBBE3C-92E3-4F42-9C19-1C3C56957249}"/>
+    <hyperlink ref="C22" r:id="rId274" display="https://codeforces.com/problemset/problem/339/A" xr:uid="{96551F71-2E9E-4AC6-9F9C-97E2DCB3CF52}"/>
+    <hyperlink ref="C23" r:id="rId275" display="https://codeforces.com/problemset/problem/1368/A" xr:uid="{F99ED325-54B8-46D6-93E7-03C0C3C97C09}"/>
+    <hyperlink ref="C24" r:id="rId276" display="https://codeforces.com/problemset/problem/702/A" xr:uid="{FA113A0B-B7E3-4281-9E47-386A37A33DF7}"/>
+    <hyperlink ref="C25" r:id="rId277" display="https://codeforces.com/problemset/problem/1097/A" xr:uid="{F8A601E3-CA87-4241-89CC-B6E33442E414}"/>
+    <hyperlink ref="C26" r:id="rId278" display="https://codeforces.com/problemset/problem/492/A" xr:uid="{4CBE06B1-8D04-4090-8270-EA81E96A8E08}"/>
+    <hyperlink ref="C27" r:id="rId279" display="https://codeforces.com/problemset/problem/1433/A" xr:uid="{2DD97C93-7A9F-4BAE-828F-8C186F977CA2}"/>
+    <hyperlink ref="C28" r:id="rId280" display="https://codeforces.com/problemset/problem/1303/A" xr:uid="{DC9A8843-7F4B-4FAA-AC48-1F393EF3605D}"/>
+    <hyperlink ref="C29" r:id="rId281" display="https://codeforces.com/problemset/problem/1095/A" xr:uid="{01DC3FA4-24F0-42F7-BD7F-9199556B2518}"/>
+    <hyperlink ref="C30" r:id="rId282" display="https://codeforces.com/problemset/problem/1391/B" xr:uid="{2B6FAAEE-6DC0-4B42-9103-232316387536}"/>
+    <hyperlink ref="C31" r:id="rId283" display="https://codeforces.com/problemset/problem/118/A" xr:uid="{44BE9B29-8D74-4DED-8F9D-02F5B4CB590B}"/>
+    <hyperlink ref="C32" r:id="rId284" display="https://codeforces.com/problemset/problem/1300/B" xr:uid="{92B64D34-EE0A-4856-B811-A6ADEA7A352A}"/>
+    <hyperlink ref="C33" r:id="rId285" display="https://codeforces.com/problemset/problem/1430/C" xr:uid="{F7CF4867-C424-448A-90E8-4EE1321388D8}"/>
+    <hyperlink ref="C34" r:id="rId286" display="https://codeforces.com/contest/139/problem/A" xr:uid="{4B633B2F-858F-4A6A-B57A-C2A220278F4B}"/>
+    <hyperlink ref="C35" r:id="rId287" display="https://codeforces.com/problemset/problem/219/A" xr:uid="{A33D8B44-D53D-4E63-885E-76AD459642EC}"/>
+    <hyperlink ref="C36" r:id="rId288" display="https://codeforces.com/problemset/problem/1141/A" xr:uid="{1000F891-8D75-4192-83AC-F3EDDB26BCD8}"/>
+    <hyperlink ref="C37" r:id="rId289" display="https://codeforces.com/problemset/problem/118/B" xr:uid="{7D5C83E1-FF95-4330-BFDF-F7000500DA5A}"/>
+    <hyperlink ref="C38" r:id="rId290" display="https://codeforces.com/problemset/problem/1373/A" xr:uid="{F56B0059-C3DC-4298-84ED-9666752DBB74}"/>
+    <hyperlink ref="C39" r:id="rId291" display="https://codeforces.com/problemset/problem/268/B" xr:uid="{3117563D-7EDB-4807-B4B2-54FA5A5A08F4}"/>
+    <hyperlink ref="C40" r:id="rId292" display="https://codeforces.com/problemset/problem/476/A" xr:uid="{4210420A-F33A-46BB-B55E-D0D4ACDCF2E1}"/>
+    <hyperlink ref="C41" r:id="rId293" display="https://codeforces.com/problemset/problem/500/A" xr:uid="{ADFEF053-1D07-4E60-8E31-EB8A4987BD51}"/>
+    <hyperlink ref="C42" r:id="rId294" display="https://codeforces.com/problemset/problem/131/A" xr:uid="{FEDDA5EC-7D82-4F5B-B3C0-3CC56B522AD4}"/>
+    <hyperlink ref="C43" r:id="rId295" display="https://codeforces.com/problemset/problem/1139/B" xr:uid="{59F9209D-68DD-44E1-A5E5-BEF79678B87C}"/>
+    <hyperlink ref="C44" r:id="rId296" display="https://codeforces.com/problemset/problem/1199/A" xr:uid="{FE2CF6F5-C5D0-47A2-A9A4-16E8195A78BF}"/>
+    <hyperlink ref="C45" r:id="rId297" display="https://codeforces.com/problemset/problem/1073/A" xr:uid="{7D1C4A7C-68EE-4BB8-8BA9-9EB897785690}"/>
+    <hyperlink ref="C46" r:id="rId298" display="https://codeforces.com/problemset/problem/109/A" xr:uid="{E2D7C15F-AC14-410F-A2C8-91C795179CDA}"/>
+    <hyperlink ref="C47" r:id="rId299" display="https://codeforces.com/problemset/problem/1244/B" xr:uid="{CE6B7CD9-584A-4E96-8104-318C23234F36}"/>
+    <hyperlink ref="C48" r:id="rId300" display="https://codeforces.com/problemset/problem/1027/A" xr:uid="{031AB86E-2C98-47B2-B573-6823BE182AE6}"/>
+    <hyperlink ref="C49" r:id="rId301" display="https://codeforces.com/problemset/problem/1278/A" xr:uid="{4F9EF49E-42DA-4C3E-956F-90F2F0F0232D}"/>
+    <hyperlink ref="C50" r:id="rId302" display="https://codeforces.com/problemset/problem/1133/A" xr:uid="{813B55F3-797D-4FA7-9EC0-DC1E5B014766}"/>
+    <hyperlink ref="C51" r:id="rId303" tooltip="Tower of Hanoi" display="https://codeforces.com/problemset/problem/507/A" xr:uid="{BABE9FB6-FCD5-4781-B412-DC2D9F4B8240}"/>
+    <hyperlink ref="C52" r:id="rId304" display="https://codeforces.com/problemset/problem/1237/A" xr:uid="{7C1C3AC5-9CBE-4E0E-BBC0-11C1A7C5BF69}"/>
+    <hyperlink ref="C53" r:id="rId305" display="https://codeforces.com/problemset/problem/486/B" xr:uid="{A854694C-E892-494E-AC84-2A19A2EF7FBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId306"/>

</xml_diff>

<commit_message>
solved constructive and implementation prob
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDA96B5-D8DD-4838-AF6B-0E5B668D473B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B6C638-67EE-461F-88C6-C39EF7B2C581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:D405"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:D30"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Solved Prob 30 Of Constructive And Implmentation
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B6C638-67EE-461F-88C6-C39EF7B2C581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1395D1B5-B266-48DC-A7FE-AEFA1AE2E0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1542,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1962,7 +1962,7 @@
         <v>33</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Sovled Implementation And Constructive Prob
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1395D1B5-B266-48DC-A7FE-AEFA1AE2E0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F48E474-2FD2-4EB3-82E8-C89C8EC7C767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:D405"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1976,7 +1976,7 @@
         <v>34</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1990,7 +1990,7 @@
         <v>35</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2004,7 +2004,7 @@
         <v>36</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
solved Constructive And Implementation Problem
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F48E474-2FD2-4EB3-82E8-C89C8EC7C767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8EE491-E25B-41E9-89C4-995F722D95EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:D405"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2018,7 +2018,7 @@
         <v>37</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2032,7 +2032,7 @@
         <v>38</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2046,7 +2046,7 @@
         <v>39</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
codeforces educational round 123
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DD3F81-606E-4BCA-982C-94CBEB9EE018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CF1047-EA8A-4289-BBBF-9D4212600A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1542,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Solved Implementation And Constructive Probelms
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC73B5E-8614-4B05-8BD6-7E3032B841E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4A5A18-163F-4A2D-AFB5-7784A996939F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1542,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1724,7 +1724,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2088,7 +2088,7 @@
         <v>42</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2130,7 +2130,7 @@
         <v>45</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2144,7 +2144,7 @@
         <v>46</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Solved PImplementation And Constructive Problem
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4A5A18-163F-4A2D-AFB5-7784A996939F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7281C4-C481-40BA-A2ED-1A6B7F490F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:D405"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2186,7 +2186,7 @@
         <v>49</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2200,7 +2200,7 @@
         <v>50</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2214,7 +2214,7 @@
         <v>51</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Solved Implementation And Constructive Problems
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7281C4-C481-40BA-A2ED-1A6B7F490F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CE5439-1012-4CCD-971E-99C3EA790DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1542,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2228,7 +2228,7 @@
         <v>52</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2242,7 +2242,7 @@
         <v>53</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2256,7 +2256,7 @@
         <v>340</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2270,7 +2270,7 @@
         <v>54</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
KickStart And Maths Problem solved
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CE5439-1012-4CCD-971E-99C3EA790DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66ACDA1-3D5B-4822-A293-A8DD16AD9CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:D405"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Solved Maths And Practice Div2 773
</commit_message>
<xml_diff>
--- a/CP Sheet/CP Sheet.xlsx
+++ b/CP Sheet/CP Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming Language\Competetive\CP Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCC2380-2C4F-491E-B022-4FCAB952F904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217A0CA3-9F22-46CD-80D3-38EB5145A6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1543,7 +1543,7 @@
   <dimension ref="A1:D405"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59:D60"/>
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2366,7 +2366,7 @@
         <v>60</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2380,7 +2380,7 @@
         <v>61</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -2394,7 +2394,7 @@
         <v>62</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>6</v>
+        <v>338</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>